<commit_message>
Auto update: 2025-10-14 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.6</v>
+        <v>2.613</v>
       </c>
       <c r="D9" t="n">
-        <v>0.97</v>
+        <v>0.5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7.725</v>
+        <v>7.775</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.004</v>
+        <v>7.059</v>
       </c>
       <c r="D11" t="n">
-        <v>2.16</v>
+        <v>0.79</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15.636</v>
+        <v>15.918</v>
       </c>
       <c r="D12" t="n">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D13" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8.867000000000001</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>3.38</v>
+        <v>1.5</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8.577</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>1.23</v>
+        <v>3.38</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21.75</v>
+        <v>22.433</v>
       </c>
       <c r="D18" t="n">
-        <v>1.52</v>
+        <v>3.14</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15.218</v>
+        <v>15.636</v>
       </c>
       <c r="D19" t="n">
-        <v>1.7</v>
+        <v>2.75</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6.856</v>
+        <v>7.004</v>
       </c>
       <c r="D20" t="n">
-        <v>1.57</v>
+        <v>2.16</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7.663</v>
+        <v>7.725</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.575</v>
+        <v>2.6</v>
       </c>
       <c r="D22" t="n">
-        <v>2.47</v>
+        <v>0.97</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -955,21 +955,21 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.076</v>
+        <v>1.086</v>
       </c>
       <c r="D23" t="n">
-        <v>1.41</v>
+        <v>0.93</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -978,21 +978,21 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D24" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1001,21 +1001,21 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6.185</v>
+        <v>6.187</v>
       </c>
       <c r="D25" t="n">
-        <v>0.41</v>
+        <v>0.03</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1024,21 +1024,21 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.568</v>
+        <v>3.593</v>
       </c>
       <c r="D26" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,203 +1061,203 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>14.573</v>
+        <v>17.782</v>
       </c>
       <c r="D28" t="n">
-        <v>1.78</v>
+        <v>1.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>7.513</v>
+        <v>21.75</v>
       </c>
       <c r="D29" t="n">
-        <v>0.85</v>
+        <v>1.52</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.96</v>
+        <v>138</v>
       </c>
       <c r="D30" t="n">
-        <v>0.74</v>
+        <v>-0.72</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6.584</v>
+        <v>8.577</v>
       </c>
       <c r="D31" t="n">
-        <v>0.61</v>
+        <v>1.23</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>21.188</v>
+        <v>15.218</v>
       </c>
       <c r="D32" t="n">
-        <v>0.71</v>
+        <v>1.7</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.475</v>
+        <v>6.856</v>
       </c>
       <c r="D33" t="n">
-        <v>1.02</v>
+        <v>1.57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.076</v>
+        <v>7.663</v>
       </c>
       <c r="D34" t="n">
-        <v>1.41</v>
+        <v>0.5</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D35" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6.185</v>
+        <v>1.076</v>
       </c>
       <c r="D36" t="n">
-        <v>0.41</v>
+        <v>1.41</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1268,214 +1268,214 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>18.7</v>
+        <v>0.96</v>
       </c>
       <c r="D37" t="n">
-        <v>0.64</v>
+        <v>0.74</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>17.782</v>
+        <v>6.185</v>
       </c>
       <c r="D38" t="n">
-        <v>1.5</v>
+        <v>0.41</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>138</v>
+        <v>3.568</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.72</v>
+        <v>0.68</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>8.327999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="D40" t="n">
-        <v>1.04</v>
+        <v>0.64</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>7.949</v>
+        <v>21.188</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9</v>
+        <v>0.71</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>7.816</v>
+        <v>2.475</v>
       </c>
       <c r="D42" t="n">
-        <v>1.82</v>
+        <v>1.02</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>7.573</v>
+        <v>14.573</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5</v>
+        <v>1.78</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>7.535</v>
+        <v>7.513</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>7.475</v>
+        <v>0.96</v>
       </c>
       <c r="D45" t="n">
-        <v>0.86</v>
+        <v>0.74</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1484,182 +1484,182 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7.349</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D46" t="n">
-        <v>2.21</v>
+        <v>1.04</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7.109</v>
+        <v>138</v>
       </c>
       <c r="D47" t="n">
-        <v>1.43</v>
+        <v>-0.72</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>7.009</v>
+        <v>17.782</v>
       </c>
       <c r="D48" t="n">
-        <v>1.18</v>
+        <v>1.5</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6.909</v>
+        <v>18.7</v>
       </c>
       <c r="D49" t="n">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6.776</v>
+        <v>6.185</v>
       </c>
       <c r="D50" t="n">
-        <v>0.73</v>
+        <v>0.41</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6.612</v>
+        <v>6.584</v>
       </c>
       <c r="D51" t="n">
-        <v>1.47</v>
+        <v>0.61</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6.325</v>
+        <v>1.076</v>
       </c>
       <c r="D52" t="n">
-        <v>0.99</v>
+        <v>1.41</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>6.231</v>
+        <v>3.568</v>
       </c>
       <c r="D53" t="n">
-        <v>0.24</v>
+        <v>0.68</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1668,21 +1668,21 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D54" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1691,21 +1691,21 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D55" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1714,21 +1714,21 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D56" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1737,21 +1737,21 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1760,21 +1760,21 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1783,21 +1783,21 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1806,21 +1806,21 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1829,21 +1829,21 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1852,21 +1852,21 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D62" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1875,21 +1875,21 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1898,21 +1898,21 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D64" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1921,21 +1921,21 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1944,35 +1944,334 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D66" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D76" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D77" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
         <v>6.167</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D80" t="n">
         <v>0</v>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-15 07:15
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.613</v>
+        <v>2.65</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5</v>
+        <v>1.42</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7.775</v>
+        <v>7.95</v>
       </c>
       <c r="D10" t="n">
-        <v>0.65</v>
+        <v>2.25</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.059</v>
+        <v>7.219</v>
       </c>
       <c r="D11" t="n">
-        <v>0.79</v>
+        <v>2.27</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>15.918</v>
+        <v>16.5</v>
       </c>
       <c r="D12" t="n">
-        <v>1.8</v>
+        <v>3.66</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>22.667</v>
+        <v>23.5</v>
       </c>
       <c r="D13" t="n">
-        <v>1.04</v>
+        <v>3.68</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>9.433</v>
       </c>
       <c r="D14" t="n">
-        <v>1.5</v>
+        <v>4.81</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8.867000000000001</v>
+        <v>9</v>
       </c>
       <c r="D17" t="n">
-        <v>3.38</v>
+        <v>1.5</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D18" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15.636</v>
+        <v>15.918</v>
       </c>
       <c r="D19" t="n">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.004</v>
+        <v>7.059</v>
       </c>
       <c r="D20" t="n">
-        <v>2.16</v>
+        <v>0.79</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7.725</v>
+        <v>7.775</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.6</v>
+        <v>2.613</v>
       </c>
       <c r="D22" t="n">
-        <v>0.97</v>
+        <v>0.5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17.782</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D28" t="n">
-        <v>1.5</v>
+        <v>3.38</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>21.75</v>
+        <v>22.433</v>
       </c>
       <c r="D29" t="n">
-        <v>1.52</v>
+        <v>3.14</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,30 +1130,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>8.577</v>
+        <v>17.782</v>
       </c>
       <c r="D31" t="n">
-        <v>1.23</v>
+        <v>1.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1162,21 +1162,21 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15.218</v>
+        <v>15.636</v>
       </c>
       <c r="D32" t="n">
-        <v>1.7</v>
+        <v>2.75</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1185,21 +1185,21 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>6.856</v>
+        <v>7.004</v>
       </c>
       <c r="D33" t="n">
-        <v>1.57</v>
+        <v>2.16</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1208,21 +1208,21 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>7.663</v>
+        <v>7.725</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1231,21 +1231,21 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.575</v>
+        <v>2.6</v>
       </c>
       <c r="D35" t="n">
-        <v>2.47</v>
+        <v>0.97</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1254,21 +1254,21 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.076</v>
+        <v>1.086</v>
       </c>
       <c r="D36" t="n">
-        <v>1.41</v>
+        <v>0.93</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1277,21 +1277,21 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D37" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1300,21 +1300,21 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6.185</v>
+        <v>6.187</v>
       </c>
       <c r="D38" t="n">
-        <v>0.41</v>
+        <v>0.03</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,21 +1323,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.568</v>
+        <v>3.593</v>
       </c>
       <c r="D39" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1360,226 +1360,226 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>21.188</v>
+        <v>15.218</v>
       </c>
       <c r="D41" t="n">
-        <v>0.71</v>
+        <v>1.7</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.475</v>
+        <v>6.856</v>
       </c>
       <c r="D42" t="n">
-        <v>1.02</v>
+        <v>1.57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>14.573</v>
+        <v>17.782</v>
       </c>
       <c r="D43" t="n">
-        <v>1.78</v>
+        <v>1.5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>7.513</v>
+        <v>21.75</v>
       </c>
       <c r="D44" t="n">
-        <v>0.85</v>
+        <v>1.52</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.96</v>
+        <v>138</v>
       </c>
       <c r="D45" t="n">
-        <v>0.74</v>
+        <v>-0.72</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>8.327999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="D46" t="n">
-        <v>1.04</v>
+        <v>0.64</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>138</v>
+        <v>3.568</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.72</v>
+        <v>0.68</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>17.782</v>
+        <v>6.185</v>
       </c>
       <c r="D48" t="n">
-        <v>1.5</v>
+        <v>0.41</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>18.7</v>
+        <v>0.96</v>
       </c>
       <c r="D49" t="n">
-        <v>0.64</v>
+        <v>0.74</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6.185</v>
+        <v>1.076</v>
       </c>
       <c r="D50" t="n">
-        <v>0.41</v>
+        <v>1.41</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1590,237 +1590,237 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>6.584</v>
+        <v>8.577</v>
       </c>
       <c r="D51" t="n">
-        <v>0.61</v>
+        <v>1.23</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.076</v>
+        <v>7.663</v>
       </c>
       <c r="D52" t="n">
-        <v>1.41</v>
+        <v>0.5</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D53" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>7.949</v>
+        <v>17.782</v>
       </c>
       <c r="D54" t="n">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>7.816</v>
+        <v>3.568</v>
       </c>
       <c r="D55" t="n">
-        <v>1.82</v>
+        <v>0.68</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>7.573</v>
+        <v>21.188</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>7.535</v>
+        <v>2.475</v>
       </c>
       <c r="D57" t="n">
-        <v>0.8</v>
+        <v>1.02</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7.475</v>
+        <v>14.573</v>
       </c>
       <c r="D58" t="n">
-        <v>0.86</v>
+        <v>1.78</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7.349</v>
+        <v>7.513</v>
       </c>
       <c r="D59" t="n">
-        <v>2.21</v>
+        <v>0.85</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>7.109</v>
+        <v>0.96</v>
       </c>
       <c r="D60" t="n">
-        <v>1.43</v>
+        <v>0.74</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1829,136 +1829,136 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>7.009</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D61" t="n">
-        <v>1.18</v>
+        <v>1.04</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>6.909</v>
+        <v>138</v>
       </c>
       <c r="D62" t="n">
-        <v>0.95</v>
+        <v>-0.72</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D63" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.612</v>
+        <v>6.185</v>
       </c>
       <c r="D64" t="n">
-        <v>1.47</v>
+        <v>0.41</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D65" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>6.231</v>
+        <v>1.076</v>
       </c>
       <c r="D66" t="n">
-        <v>0.24</v>
+        <v>1.41</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1967,21 +1967,21 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D67" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1990,21 +1990,21 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D68" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2013,21 +2013,21 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D69" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2036,21 +2036,21 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2059,21 +2059,21 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2082,21 +2082,21 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2105,21 +2105,21 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2128,21 +2128,21 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2151,21 +2151,21 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D75" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2174,21 +2174,21 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2197,21 +2197,21 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2220,21 +2220,21 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2243,35 +2243,334 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D89" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D90" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D91" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D92" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
-        </is>
-      </c>
-      <c r="C80" t="n">
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
         <v>6.167</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D93" t="n">
         <v>0</v>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-16 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.65</v>
+        <v>2.7</v>
       </c>
       <c r="D9" t="n">
-        <v>1.42</v>
+        <v>1.89</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7.95</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>2.25</v>
+        <v>1.57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.219</v>
+        <v>7.522</v>
       </c>
       <c r="D11" t="n">
-        <v>2.27</v>
+        <v>4.2</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>16.5</v>
+        <v>17.055</v>
       </c>
       <c r="D12" t="n">
-        <v>3.66</v>
+        <v>3.36</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>23.5</v>
+        <v>23.833</v>
       </c>
       <c r="D13" t="n">
-        <v>3.68</v>
+        <v>1.42</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9.433</v>
+        <v>9.715</v>
       </c>
       <c r="D14" t="n">
-        <v>4.81</v>
+        <v>3.72</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>9.433</v>
       </c>
       <c r="D17" t="n">
-        <v>1.5</v>
+        <v>4.81</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>22.667</v>
+        <v>23.5</v>
       </c>
       <c r="D18" t="n">
-        <v>1.04</v>
+        <v>3.68</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>15.918</v>
+        <v>16.5</v>
       </c>
       <c r="D19" t="n">
-        <v>1.8</v>
+        <v>3.66</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.059</v>
+        <v>7.219</v>
       </c>
       <c r="D20" t="n">
-        <v>0.79</v>
+        <v>2.27</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7.775</v>
+        <v>7.95</v>
       </c>
       <c r="D21" t="n">
-        <v>0.65</v>
+        <v>2.25</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.613</v>
+        <v>2.65</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5</v>
+        <v>1.42</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>8.867000000000001</v>
+        <v>17.782</v>
       </c>
       <c r="D28" t="n">
-        <v>3.38</v>
+        <v>1.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D29" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,134 +1130,134 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17.782</v>
+        <v>9</v>
       </c>
       <c r="D31" t="n">
         <v>1.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15.636</v>
+        <v>7.059</v>
       </c>
       <c r="D32" t="n">
-        <v>2.75</v>
+        <v>0.79</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7.004</v>
+        <v>7.775</v>
       </c>
       <c r="D33" t="n">
-        <v>2.16</v>
+        <v>0.65</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>7.725</v>
+        <v>18.7</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.6</v>
+        <v>3.593</v>
       </c>
       <c r="D35" t="n">
-        <v>0.97</v>
+        <v>0.7</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.086</v>
+        <v>6.187</v>
       </c>
       <c r="D36" t="n">
-        <v>0.93</v>
+        <v>0.03</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1291,19 +1291,19 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D38" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1314,76 +1314,76 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.593</v>
+        <v>15.918</v>
       </c>
       <c r="D39" t="n">
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>18.7</v>
+        <v>2.613</v>
       </c>
       <c r="D40" t="n">
-        <v>0.64</v>
+        <v>0.5</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>15.218</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D41" t="n">
-        <v>1.7</v>
+        <v>3.38</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1392,79 +1392,79 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>6.856</v>
+        <v>7.004</v>
       </c>
       <c r="D42" t="n">
-        <v>1.57</v>
+        <v>2.16</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>17.782</v>
+        <v>15.636</v>
       </c>
       <c r="D43" t="n">
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>21.75</v>
+        <v>138</v>
       </c>
       <c r="D44" t="n">
-        <v>1.52</v>
+        <v>-0.72</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>138</v>
+        <v>17.782</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.72</v>
+        <v>1.5</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1475,7 +1475,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1498,7 +1498,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1507,21 +1507,21 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.568</v>
+        <v>3.593</v>
       </c>
       <c r="D47" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1530,21 +1530,21 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>6.185</v>
+        <v>6.187</v>
       </c>
       <c r="D48" t="n">
-        <v>0.41</v>
+        <v>0.03</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1553,21 +1553,21 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D49" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1576,44 +1576,44 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.076</v>
+        <v>1.086</v>
       </c>
       <c r="D50" t="n">
-        <v>1.41</v>
+        <v>0.93</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>8.577</v>
+        <v>2.6</v>
       </c>
       <c r="D51" t="n">
-        <v>1.23</v>
+        <v>0.97</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1622,194 +1622,194 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7.663</v>
+        <v>7.725</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2.575</v>
+        <v>22.433</v>
       </c>
       <c r="D53" t="n">
-        <v>2.47</v>
+        <v>3.14</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>17.782</v>
+        <v>0.96</v>
       </c>
       <c r="D54" t="n">
-        <v>1.5</v>
+        <v>0.74</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D55" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>21.188</v>
+        <v>7.663</v>
       </c>
       <c r="D56" t="n">
-        <v>0.71</v>
+        <v>0.5</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.475</v>
+        <v>8.577</v>
       </c>
       <c r="D57" t="n">
-        <v>1.02</v>
+        <v>1.23</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>14.573</v>
+        <v>1.076</v>
       </c>
       <c r="D58" t="n">
-        <v>1.78</v>
+        <v>1.41</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7.513</v>
+        <v>6.185</v>
       </c>
       <c r="D59" t="n">
-        <v>0.85</v>
+        <v>0.41</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.96</v>
+        <v>3.568</v>
       </c>
       <c r="D60" t="n">
-        <v>0.74</v>
+        <v>0.68</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1820,30 +1820,30 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>8.327999999999999</v>
+        <v>18.7</v>
       </c>
       <c r="D61" t="n">
-        <v>1.04</v>
+        <v>0.64</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1866,283 +1866,283 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>18.7</v>
+        <v>21.75</v>
       </c>
       <c r="D63" t="n">
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D64" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.584</v>
+        <v>15.218</v>
       </c>
       <c r="D65" t="n">
-        <v>0.61</v>
+        <v>1.7</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.076</v>
+        <v>6.856</v>
       </c>
       <c r="D66" t="n">
-        <v>1.41</v>
+        <v>1.57</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>7.949</v>
+        <v>138</v>
       </c>
       <c r="D67" t="n">
-        <v>0.9</v>
+        <v>-0.72</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>7.816</v>
+        <v>17.782</v>
       </c>
       <c r="D68" t="n">
-        <v>1.82</v>
+        <v>1.5</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>7.573</v>
+        <v>3.568</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>7.535</v>
+        <v>21.188</v>
       </c>
       <c r="D70" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>7.475</v>
+        <v>2.475</v>
       </c>
       <c r="D71" t="n">
-        <v>0.86</v>
+        <v>1.02</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>7.349</v>
+        <v>14.573</v>
       </c>
       <c r="D72" t="n">
-        <v>2.21</v>
+        <v>1.78</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7.109</v>
+        <v>7.513</v>
       </c>
       <c r="D73" t="n">
-        <v>1.43</v>
+        <v>0.85</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7.009</v>
+        <v>0.96</v>
       </c>
       <c r="D74" t="n">
-        <v>1.18</v>
+        <v>0.74</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2151,113 +2151,113 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6.909</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D75" t="n">
-        <v>0.95</v>
+        <v>1.04</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D76" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>6.612</v>
+        <v>6.185</v>
       </c>
       <c r="D77" t="n">
-        <v>1.47</v>
+        <v>0.41</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D78" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.231</v>
+        <v>1.076</v>
       </c>
       <c r="D79" t="n">
-        <v>0.24</v>
+        <v>1.41</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2266,21 +2266,21 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D80" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2289,21 +2289,21 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D81" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2312,21 +2312,21 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D82" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2335,21 +2335,21 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2358,21 +2358,21 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2381,21 +2381,21 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2404,21 +2404,21 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2427,21 +2427,21 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2450,21 +2450,21 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D88" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2473,21 +2473,21 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2496,21 +2496,21 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2519,21 +2519,21 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2542,35 +2542,334 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D102" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D103" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D104" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D105" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
-        </is>
-      </c>
-      <c r="C93" t="n">
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
         <v>6.167</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D106" t="n">
         <v>0</v>
       </c>
-      <c r="E93" t="inlineStr">
+      <c r="E106" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-17 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.7</v>
+        <v>2.72</v>
       </c>
       <c r="D9" t="n">
-        <v>1.89</v>
+        <v>0.74</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.074999999999999</v>
+        <v>8.25</v>
       </c>
       <c r="D10" t="n">
-        <v>1.57</v>
+        <v>2.17</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.522</v>
+        <v>7.946</v>
       </c>
       <c r="D11" t="n">
-        <v>4.2</v>
+        <v>4.98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17.055</v>
+        <v>17.909</v>
       </c>
       <c r="D12" t="n">
-        <v>3.36</v>
+        <v>5.01</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>23.833</v>
+        <v>24.167</v>
       </c>
       <c r="D13" t="n">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9.715</v>
+        <v>10.343</v>
       </c>
       <c r="D14" t="n">
-        <v>3.72</v>
+        <v>5.69</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9.433</v>
+        <v>9.715</v>
       </c>
       <c r="D17" t="n">
-        <v>4.81</v>
+        <v>3.72</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>23.5</v>
+        <v>23.833</v>
       </c>
       <c r="D18" t="n">
-        <v>3.68</v>
+        <v>1.42</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>16.5</v>
+        <v>17.055</v>
       </c>
       <c r="D19" t="n">
-        <v>3.66</v>
+        <v>3.36</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.219</v>
+        <v>7.522</v>
       </c>
       <c r="D20" t="n">
-        <v>2.27</v>
+        <v>4.2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>7.95</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D21" t="n">
-        <v>2.25</v>
+        <v>1.57</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.65</v>
+        <v>2.7</v>
       </c>
       <c r="D22" t="n">
-        <v>1.42</v>
+        <v>1.89</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17.782</v>
+        <v>9.433</v>
       </c>
       <c r="D28" t="n">
-        <v>1.5</v>
+        <v>4.81</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>22.667</v>
+        <v>23.5</v>
       </c>
       <c r="D29" t="n">
-        <v>1.04</v>
+        <v>3.68</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,30 +1130,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9</v>
+        <v>17.782</v>
       </c>
       <c r="D31" t="n">
         <v>1.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1162,21 +1162,21 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7.059</v>
+        <v>7.219</v>
       </c>
       <c r="D32" t="n">
-        <v>0.79</v>
+        <v>2.27</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1185,21 +1185,21 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7.775</v>
+        <v>7.95</v>
       </c>
       <c r="D33" t="n">
-        <v>0.65</v>
+        <v>2.25</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1291,7 +1291,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1314,7 +1314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,21 +1323,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>15.918</v>
+        <v>16.5</v>
       </c>
       <c r="D39" t="n">
-        <v>1.8</v>
+        <v>3.66</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1346,90 +1346,90 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2.613</v>
+        <v>2.65</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5</v>
+        <v>1.42</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>8.867000000000001</v>
+        <v>17.782</v>
       </c>
       <c r="D41" t="n">
-        <v>3.38</v>
+        <v>1.5</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>7.004</v>
+        <v>7.775</v>
       </c>
       <c r="D42" t="n">
-        <v>2.16</v>
+        <v>0.65</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>15.636</v>
+        <v>7.059</v>
       </c>
       <c r="D43" t="n">
-        <v>2.75</v>
+        <v>0.79</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1452,88 +1452,88 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17.782</v>
+        <v>9</v>
       </c>
       <c r="D45" t="n">
         <v>1.5</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>18.7</v>
+        <v>2.613</v>
       </c>
       <c r="D46" t="n">
-        <v>0.64</v>
+        <v>0.5</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.593</v>
+        <v>15.918</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D48" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1544,7 +1544,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,19 +1567,19 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.086</v>
+        <v>6.187</v>
       </c>
       <c r="D50" t="n">
-        <v>0.93</v>
+        <v>0.03</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1590,53 +1590,53 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2.6</v>
+        <v>3.593</v>
       </c>
       <c r="D51" t="n">
-        <v>0.97</v>
+        <v>0.7</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7.725</v>
+        <v>18.7</v>
       </c>
       <c r="D52" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1645,21 +1645,21 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D53" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1668,44 +1668,44 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D54" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2.575</v>
+        <v>22.433</v>
       </c>
       <c r="D55" t="n">
-        <v>2.47</v>
+        <v>3.14</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1714,44 +1714,44 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>7.663</v>
+        <v>7.725</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>8.577</v>
+        <v>2.6</v>
       </c>
       <c r="D57" t="n">
-        <v>1.23</v>
+        <v>0.97</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1760,21 +1760,21 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1.076</v>
+        <v>1.086</v>
       </c>
       <c r="D58" t="n">
-        <v>1.41</v>
+        <v>0.93</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1783,21 +1783,21 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>6.185</v>
+        <v>6.187</v>
       </c>
       <c r="D59" t="n">
-        <v>0.41</v>
+        <v>0.03</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1806,21 +1806,21 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>3.568</v>
+        <v>3.593</v>
       </c>
       <c r="D60" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1843,19 +1843,19 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>138</v>
+        <v>17.782</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.72</v>
+        <v>1.5</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1866,76 +1866,76 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>21.75</v>
+        <v>138</v>
       </c>
       <c r="D63" t="n">
-        <v>1.52</v>
+        <v>-0.72</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>17.782</v>
+        <v>15.636</v>
       </c>
       <c r="D64" t="n">
-        <v>1.5</v>
+        <v>2.75</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>15.218</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D65" t="n">
-        <v>1.7</v>
+        <v>3.38</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1944,33 +1944,33 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>6.856</v>
+        <v>7.004</v>
       </c>
       <c r="D66" t="n">
-        <v>1.57</v>
+        <v>2.16</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>138</v>
+        <v>18.7</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.72</v>
+        <v>0.64</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -1981,157 +1981,157 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>17.782</v>
+        <v>0.96</v>
       </c>
       <c r="D68" t="n">
-        <v>1.5</v>
+        <v>0.74</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D69" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>21.188</v>
+        <v>7.663</v>
       </c>
       <c r="D70" t="n">
-        <v>0.71</v>
+        <v>0.5</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2.475</v>
+        <v>8.577</v>
       </c>
       <c r="D71" t="n">
-        <v>1.02</v>
+        <v>1.23</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>14.573</v>
+        <v>1.076</v>
       </c>
       <c r="D72" t="n">
-        <v>1.78</v>
+        <v>1.41</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7.513</v>
+        <v>6.185</v>
       </c>
       <c r="D73" t="n">
-        <v>0.85</v>
+        <v>0.41</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.96</v>
+        <v>3.568</v>
       </c>
       <c r="D74" t="n">
-        <v>0.74</v>
+        <v>0.68</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2142,329 +2142,329 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8.327999999999999</v>
+        <v>138</v>
       </c>
       <c r="D75" t="n">
-        <v>1.04</v>
+        <v>-0.72</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>18.7</v>
+        <v>21.75</v>
       </c>
       <c r="D76" t="n">
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D77" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.584</v>
+        <v>15.218</v>
       </c>
       <c r="D78" t="n">
-        <v>0.61</v>
+        <v>1.7</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.076</v>
+        <v>6.856</v>
       </c>
       <c r="D79" t="n">
-        <v>1.41</v>
+        <v>1.57</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>7.949</v>
+        <v>138</v>
       </c>
       <c r="D80" t="n">
-        <v>0.9</v>
+        <v>-0.72</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7.816</v>
+        <v>3.568</v>
       </c>
       <c r="D81" t="n">
-        <v>1.82</v>
+        <v>0.68</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>7.573</v>
+        <v>17.782</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>7.535</v>
+        <v>21.188</v>
       </c>
       <c r="D83" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.475</v>
+        <v>2.475</v>
       </c>
       <c r="D84" t="n">
-        <v>0.86</v>
+        <v>1.02</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7.349</v>
+        <v>1.076</v>
       </c>
       <c r="D85" t="n">
-        <v>2.21</v>
+        <v>1.41</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7.109</v>
+        <v>6.584</v>
       </c>
       <c r="D86" t="n">
-        <v>1.43</v>
+        <v>0.61</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7.009</v>
+        <v>6.185</v>
       </c>
       <c r="D87" t="n">
-        <v>1.18</v>
+        <v>0.41</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6.909</v>
+        <v>18.7</v>
       </c>
       <c r="D88" t="n">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2473,90 +2473,90 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>6.776</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D89" t="n">
-        <v>0.73</v>
+        <v>1.04</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>6.612</v>
+        <v>0.96</v>
       </c>
       <c r="D90" t="n">
-        <v>1.47</v>
+        <v>0.74</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>6.325</v>
+        <v>7.513</v>
       </c>
       <c r="D91" t="n">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6.231</v>
+        <v>14.573</v>
       </c>
       <c r="D92" t="n">
-        <v>0.24</v>
+        <v>1.78</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2565,21 +2565,21 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D93" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2588,21 +2588,21 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D94" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2611,21 +2611,21 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D95" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2634,21 +2634,21 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2657,21 +2657,21 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2680,21 +2680,21 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2703,21 +2703,21 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2726,21 +2726,21 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2749,21 +2749,21 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D101" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2772,21 +2772,21 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D102" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2795,21 +2795,21 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D103" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2818,21 +2818,21 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D104" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2841,35 +2841,334 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D115" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D116" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D117" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D118" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
         <v>6.167</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D119" t="n">
         <v>0</v>
       </c>
-      <c r="E106" t="inlineStr">
+      <c r="E119" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-18 07:12
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -640,14 +640,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -663,14 +663,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D11" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -709,14 +709,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -732,14 +732,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -755,14 +755,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9.715</v>
+        <v>10.343</v>
       </c>
       <c r="D17" t="n">
-        <v>3.72</v>
+        <v>5.69</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>23.833</v>
+        <v>24.167</v>
       </c>
       <c r="D18" t="n">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17.055</v>
+        <v>17.909</v>
       </c>
       <c r="D19" t="n">
-        <v>3.36</v>
+        <v>5.01</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.522</v>
+        <v>7.946</v>
       </c>
       <c r="D20" t="n">
-        <v>4.2</v>
+        <v>4.98</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.074999999999999</v>
+        <v>8.25</v>
       </c>
       <c r="D21" t="n">
-        <v>1.57</v>
+        <v>2.17</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.7</v>
+        <v>2.72</v>
       </c>
       <c r="D22" t="n">
-        <v>1.89</v>
+        <v>0.74</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9.433</v>
+        <v>17.782</v>
       </c>
       <c r="D28" t="n">
-        <v>4.81</v>
+        <v>1.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23.5</v>
+        <v>23.833</v>
       </c>
       <c r="D29" t="n">
-        <v>3.68</v>
+        <v>1.42</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,76 +1130,76 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17.782</v>
+        <v>9.715</v>
       </c>
       <c r="D31" t="n">
-        <v>1.5</v>
+        <v>3.72</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>7.219</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D32" t="n">
-        <v>2.27</v>
+        <v>1.57</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7.95</v>
+        <v>2.7</v>
       </c>
       <c r="D33" t="n">
-        <v>2.25</v>
+        <v>1.89</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1291,191 +1291,191 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1.086</v>
+        <v>17.055</v>
       </c>
       <c r="D38" t="n">
-        <v>0.93</v>
+        <v>3.36</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>16.5</v>
+        <v>7.522</v>
       </c>
       <c r="D39" t="n">
-        <v>3.66</v>
+        <v>4.2</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2.65</v>
+        <v>1.086</v>
       </c>
       <c r="D40" t="n">
-        <v>1.42</v>
+        <v>0.93</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>17.782</v>
+        <v>23.5</v>
       </c>
       <c r="D41" t="n">
-        <v>1.5</v>
+        <v>3.68</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>7.775</v>
+        <v>9.433</v>
       </c>
       <c r="D42" t="n">
-        <v>0.65</v>
+        <v>4.81</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>7.059</v>
+        <v>17.782</v>
       </c>
       <c r="D43" t="n">
-        <v>0.79</v>
+        <v>1.5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>138</v>
+        <v>7.219</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.72</v>
+        <v>2.27</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>9</v>
+        <v>7.95</v>
       </c>
       <c r="D45" t="n">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1484,21 +1484,21 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2.613</v>
+        <v>2.65</v>
       </c>
       <c r="D46" t="n">
-        <v>0.5</v>
+        <v>1.42</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1507,21 +1507,21 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>15.918</v>
+        <v>16.5</v>
       </c>
       <c r="D47" t="n">
-        <v>1.8</v>
+        <v>3.66</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1544,7 +1544,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1590,7 +1590,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1613,7 +1613,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1636,42 +1636,42 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>22.667</v>
+        <v>138</v>
       </c>
       <c r="D53" t="n">
-        <v>1.04</v>
+        <v>-0.72</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.972</v>
+        <v>1.086</v>
       </c>
       <c r="D54" t="n">
-        <v>1.25</v>
+        <v>0.93</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1682,7 +1682,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1691,297 +1691,297 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D55" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>7.725</v>
+        <v>18.7</v>
       </c>
       <c r="D56" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.6</v>
+        <v>17.782</v>
       </c>
       <c r="D57" t="n">
-        <v>0.97</v>
+        <v>1.5</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1.086</v>
+        <v>7.775</v>
       </c>
       <c r="D58" t="n">
-        <v>0.93</v>
+        <v>0.65</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>6.187</v>
+        <v>7.059</v>
       </c>
       <c r="D59" t="n">
-        <v>0.03</v>
+        <v>0.79</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>3.593</v>
+        <v>138</v>
       </c>
       <c r="D60" t="n">
-        <v>0.7</v>
+        <v>-0.72</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>18.7</v>
+        <v>9</v>
       </c>
       <c r="D61" t="n">
-        <v>0.64</v>
+        <v>1.5</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>17.782</v>
+        <v>2.613</v>
       </c>
       <c r="D62" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>138</v>
+        <v>15.918</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.72</v>
+        <v>1.8</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>15.636</v>
+        <v>0.972</v>
       </c>
       <c r="D64" t="n">
-        <v>2.75</v>
+        <v>1.25</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>8.867000000000001</v>
+        <v>6.187</v>
       </c>
       <c r="D65" t="n">
-        <v>3.38</v>
+        <v>0.03</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7.004</v>
+        <v>3.593</v>
       </c>
       <c r="D66" t="n">
-        <v>2.16</v>
+        <v>0.7</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>18.7</v>
+        <v>22.433</v>
       </c>
       <c r="D67" t="n">
-        <v>0.64</v>
+        <v>3.14</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1990,274 +1990,274 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D68" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2.575</v>
+        <v>7.004</v>
       </c>
       <c r="D69" t="n">
-        <v>2.47</v>
+        <v>2.16</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>7.663</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5</v>
+        <v>3.38</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>8.577</v>
+        <v>15.636</v>
       </c>
       <c r="D71" t="n">
-        <v>1.23</v>
+        <v>2.75</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.076</v>
+        <v>138</v>
       </c>
       <c r="D72" t="n">
-        <v>1.41</v>
+        <v>-0.72</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D73" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3.568</v>
+        <v>18.7</v>
       </c>
       <c r="D74" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>138</v>
+        <v>3.593</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>21.75</v>
+        <v>6.187</v>
       </c>
       <c r="D76" t="n">
-        <v>1.52</v>
+        <v>0.03</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>17.782</v>
+        <v>1.086</v>
       </c>
       <c r="D77" t="n">
-        <v>1.5</v>
+        <v>0.93</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>15.218</v>
+        <v>2.6</v>
       </c>
       <c r="D78" t="n">
-        <v>1.7</v>
+        <v>0.97</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.856</v>
+        <v>7.725</v>
       </c>
       <c r="D79" t="n">
-        <v>1.57</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2280,145 +2280,145 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3.568</v>
+        <v>18.7</v>
       </c>
       <c r="D81" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>17.782</v>
+        <v>0.96</v>
       </c>
       <c r="D82" t="n">
-        <v>1.5</v>
+        <v>0.74</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>21.188</v>
+        <v>2.575</v>
       </c>
       <c r="D83" t="n">
-        <v>0.71</v>
+        <v>2.47</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2.475</v>
+        <v>7.663</v>
       </c>
       <c r="D84" t="n">
-        <v>1.02</v>
+        <v>0.5</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1.076</v>
+        <v>8.577</v>
       </c>
       <c r="D85" t="n">
-        <v>1.41</v>
+        <v>1.23</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>6.584</v>
+        <v>1.076</v>
       </c>
       <c r="D86" t="n">
-        <v>0.61</v>
+        <v>1.41</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2441,306 +2441,306 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>18.7</v>
+        <v>3.568</v>
       </c>
       <c r="D88" t="n">
-        <v>0.64</v>
+        <v>0.68</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8.327999999999999</v>
+        <v>21.75</v>
       </c>
       <c r="D89" t="n">
-        <v>1.04</v>
+        <v>1.52</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.96</v>
+        <v>17.782</v>
       </c>
       <c r="D90" t="n">
-        <v>0.74</v>
+        <v>1.5</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>7.513</v>
+        <v>15.218</v>
       </c>
       <c r="D91" t="n">
-        <v>0.85</v>
+        <v>1.7</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>14.573</v>
+        <v>6.856</v>
       </c>
       <c r="D92" t="n">
-        <v>1.78</v>
+        <v>1.57</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>7.949</v>
+        <v>17.782</v>
       </c>
       <c r="D93" t="n">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>7.816</v>
+        <v>138</v>
       </c>
       <c r="D94" t="n">
-        <v>1.82</v>
+        <v>-0.72</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7.573</v>
+        <v>3.568</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7.535</v>
+        <v>21.188</v>
       </c>
       <c r="D96" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7.475</v>
+        <v>2.475</v>
       </c>
       <c r="D97" t="n">
-        <v>0.86</v>
+        <v>1.02</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7.349</v>
+        <v>14.573</v>
       </c>
       <c r="D98" t="n">
-        <v>2.21</v>
+        <v>1.78</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7.109</v>
+        <v>7.513</v>
       </c>
       <c r="D99" t="n">
-        <v>1.43</v>
+        <v>0.85</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>7.009</v>
+        <v>0.96</v>
       </c>
       <c r="D100" t="n">
-        <v>1.18</v>
+        <v>0.74</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2749,113 +2749,113 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>6.909</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D101" t="n">
-        <v>0.95</v>
+        <v>1.04</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D102" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>6.612</v>
+        <v>6.185</v>
       </c>
       <c r="D103" t="n">
-        <v>1.47</v>
+        <v>0.41</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D104" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>6.231</v>
+        <v>1.076</v>
       </c>
       <c r="D105" t="n">
-        <v>0.24</v>
+        <v>1.41</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2864,21 +2864,21 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D106" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2887,21 +2887,21 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D107" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2910,21 +2910,21 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D108" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2933,21 +2933,21 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2956,21 +2956,21 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2979,21 +2979,21 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -3002,21 +3002,21 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3025,21 +3025,21 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3048,21 +3048,21 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D114" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3071,21 +3071,21 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D115" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -3094,21 +3094,21 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D116" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -3117,21 +3117,21 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D117" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3140,35 +3140,334 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D118" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D129" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
+      <c r="B132" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C119" t="n">
+      <c r="C132" t="n">
         <v>6.167</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D132" t="n">
         <v>0</v>
       </c>
-      <c r="E119" t="inlineStr">
+      <c r="E132" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-19 07:12
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -647,7 +647,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -670,7 +670,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -693,7 +693,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -739,7 +739,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -762,7 +762,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -824,14 +824,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -847,14 +847,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -870,14 +870,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D20" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -916,14 +916,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -939,14 +939,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D28" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23.833</v>
+        <v>24.167</v>
       </c>
       <c r="D29" t="n">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,30 +1130,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9.715</v>
+        <v>17.782</v>
       </c>
       <c r="D31" t="n">
-        <v>3.72</v>
+        <v>1.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1162,21 +1162,21 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8.074999999999999</v>
+        <v>8.25</v>
       </c>
       <c r="D32" t="n">
-        <v>1.57</v>
+        <v>2.17</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1185,21 +1185,21 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.7</v>
+        <v>2.72</v>
       </c>
       <c r="D33" t="n">
-        <v>1.89</v>
+        <v>0.74</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1291,7 +1291,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1300,21 +1300,21 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>17.055</v>
+        <v>17.909</v>
       </c>
       <c r="D38" t="n">
-        <v>3.36</v>
+        <v>5.01</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,21 +1323,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.522</v>
+        <v>7.946</v>
       </c>
       <c r="D39" t="n">
-        <v>4.2</v>
+        <v>4.98</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1360,7 +1360,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1369,182 +1369,182 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>23.5</v>
+        <v>23.833</v>
       </c>
       <c r="D41" t="n">
-        <v>3.68</v>
+        <v>1.42</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>9.433</v>
+        <v>17.782</v>
       </c>
       <c r="D42" t="n">
-        <v>4.81</v>
+        <v>1.5</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>17.782</v>
+        <v>9.715</v>
       </c>
       <c r="D43" t="n">
-        <v>1.5</v>
+        <v>3.72</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>7.219</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D44" t="n">
-        <v>2.27</v>
+        <v>1.57</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>7.95</v>
+        <v>2.7</v>
       </c>
       <c r="D45" t="n">
-        <v>2.25</v>
+        <v>1.89</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2.65</v>
+        <v>1.086</v>
       </c>
       <c r="D46" t="n">
-        <v>1.42</v>
+        <v>0.93</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>16.5</v>
+        <v>7.522</v>
       </c>
       <c r="D47" t="n">
-        <v>3.66</v>
+        <v>4.2</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.086</v>
+        <v>17.055</v>
       </c>
       <c r="D48" t="n">
-        <v>0.93</v>
+        <v>3.36</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1590,7 +1590,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1613,7 +1613,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1659,7 +1659,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1682,30 +1682,30 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>22.667</v>
+        <v>138</v>
       </c>
       <c r="D55" t="n">
-        <v>1.04</v>
+        <v>-0.72</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1728,122 +1728,122 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>17.782</v>
+        <v>23.5</v>
       </c>
       <c r="D57" t="n">
-        <v>1.5</v>
+        <v>3.68</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>7.775</v>
+        <v>9.433</v>
       </c>
       <c r="D58" t="n">
-        <v>0.65</v>
+        <v>4.81</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7.059</v>
+        <v>17.782</v>
       </c>
       <c r="D59" t="n">
-        <v>0.79</v>
+        <v>1.5</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>138</v>
+        <v>7.219</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.72</v>
+        <v>2.27</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>7.95</v>
       </c>
       <c r="D61" t="n">
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1852,21 +1852,21 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.613</v>
+        <v>2.65</v>
       </c>
       <c r="D62" t="n">
-        <v>0.5</v>
+        <v>1.42</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1875,21 +1875,21 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>15.918</v>
+        <v>16.5</v>
       </c>
       <c r="D63" t="n">
-        <v>1.8</v>
+        <v>3.66</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1935,7 +1935,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1958,7 +1958,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1967,33 +1967,33 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>22.433</v>
+        <v>22.667</v>
       </c>
       <c r="D67" t="n">
-        <v>3.14</v>
+        <v>1.04</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.972</v>
+        <v>1.086</v>
       </c>
       <c r="D68" t="n">
-        <v>1.25</v>
+        <v>0.93</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2004,272 +2004,272 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>7.004</v>
+        <v>3.593</v>
       </c>
       <c r="D69" t="n">
-        <v>2.16</v>
+        <v>0.7</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>8.867000000000001</v>
+        <v>6.187</v>
       </c>
       <c r="D70" t="n">
-        <v>3.38</v>
+        <v>0.03</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>15.636</v>
+        <v>0.972</v>
       </c>
       <c r="D71" t="n">
-        <v>2.75</v>
+        <v>1.25</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>138</v>
+        <v>15.918</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.72</v>
+        <v>1.8</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>17.782</v>
+        <v>2.613</v>
       </c>
       <c r="D73" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>18.7</v>
+        <v>9</v>
       </c>
       <c r="D74" t="n">
-        <v>0.64</v>
+        <v>1.5</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3.593</v>
+        <v>138</v>
       </c>
       <c r="D75" t="n">
-        <v>0.7</v>
+        <v>-0.72</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>6.187</v>
+        <v>7.059</v>
       </c>
       <c r="D76" t="n">
-        <v>0.03</v>
+        <v>0.79</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1.086</v>
+        <v>7.775</v>
       </c>
       <c r="D77" t="n">
-        <v>0.93</v>
+        <v>0.65</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.6</v>
+        <v>17.782</v>
       </c>
       <c r="D78" t="n">
-        <v>0.97</v>
+        <v>1.5</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>7.725</v>
+        <v>18.7</v>
       </c>
       <c r="D79" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>138</v>
+        <v>18.7</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.72</v>
+        <v>0.64</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2280,30 +2280,30 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>18.7</v>
+        <v>22.433</v>
       </c>
       <c r="D81" t="n">
-        <v>0.64</v>
+        <v>3.14</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2312,136 +2312,136 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D82" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>2.575</v>
+        <v>7.004</v>
       </c>
       <c r="D83" t="n">
-        <v>2.47</v>
+        <v>2.16</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.663</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5</v>
+        <v>3.38</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>8.577</v>
+        <v>15.636</v>
       </c>
       <c r="D85" t="n">
-        <v>1.23</v>
+        <v>2.75</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.076</v>
+        <v>138</v>
       </c>
       <c r="D86" t="n">
-        <v>1.41</v>
+        <v>-0.72</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D87" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2450,125 +2450,125 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3.568</v>
+        <v>3.593</v>
       </c>
       <c r="D88" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>21.75</v>
+        <v>6.187</v>
       </c>
       <c r="D89" t="n">
-        <v>1.52</v>
+        <v>0.03</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>17.782</v>
+        <v>1.086</v>
       </c>
       <c r="D90" t="n">
-        <v>1.5</v>
+        <v>0.93</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>15.218</v>
+        <v>2.6</v>
       </c>
       <c r="D91" t="n">
-        <v>1.7</v>
+        <v>0.97</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6.856</v>
+        <v>7.725</v>
       </c>
       <c r="D92" t="n">
-        <v>1.57</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>17.782</v>
+        <v>138</v>
       </c>
       <c r="D93" t="n">
-        <v>1.5</v>
+        <v>-0.72</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2579,157 +2579,157 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>138</v>
+        <v>0.96</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.72</v>
+        <v>0.74</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>3.568</v>
+        <v>18.7</v>
       </c>
       <c r="D95" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>21.188</v>
+        <v>6.856</v>
       </c>
       <c r="D96" t="n">
-        <v>0.71</v>
+        <v>1.57</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>2.475</v>
+        <v>15.218</v>
       </c>
       <c r="D97" t="n">
-        <v>1.02</v>
+        <v>1.7</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>14.573</v>
+        <v>17.782</v>
       </c>
       <c r="D98" t="n">
-        <v>1.78</v>
+        <v>1.5</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7.513</v>
+        <v>21.75</v>
       </c>
       <c r="D99" t="n">
-        <v>0.85</v>
+        <v>1.52</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.96</v>
+        <v>3.568</v>
       </c>
       <c r="D100" t="n">
-        <v>0.74</v>
+        <v>0.68</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2740,329 +2740,329 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8.327999999999999</v>
+        <v>6.185</v>
       </c>
       <c r="D101" t="n">
-        <v>1.04</v>
+        <v>0.41</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>18.7</v>
+        <v>1.076</v>
       </c>
       <c r="D102" t="n">
-        <v>0.64</v>
+        <v>1.41</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>6.185</v>
+        <v>8.577</v>
       </c>
       <c r="D103" t="n">
-        <v>0.41</v>
+        <v>1.23</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6.584</v>
+        <v>7.663</v>
       </c>
       <c r="D104" t="n">
-        <v>0.61</v>
+        <v>0.5</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1.076</v>
+        <v>2.575</v>
       </c>
       <c r="D105" t="n">
-        <v>1.41</v>
+        <v>2.47</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>7.949</v>
+        <v>21.188</v>
       </c>
       <c r="D106" t="n">
-        <v>0.9</v>
+        <v>0.71</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>7.816</v>
+        <v>138</v>
       </c>
       <c r="D107" t="n">
-        <v>1.82</v>
+        <v>-0.72</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>7.573</v>
+        <v>2.475</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5</v>
+        <v>1.02</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>7.535</v>
+        <v>3.568</v>
       </c>
       <c r="D109" t="n">
-        <v>0.8</v>
+        <v>0.68</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>7.475</v>
+        <v>17.782</v>
       </c>
       <c r="D110" t="n">
-        <v>0.86</v>
+        <v>1.5</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>7.349</v>
+        <v>1.076</v>
       </c>
       <c r="D111" t="n">
-        <v>2.21</v>
+        <v>1.41</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>7.109</v>
+        <v>6.584</v>
       </c>
       <c r="D112" t="n">
-        <v>1.43</v>
+        <v>0.61</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>7.009</v>
+        <v>6.185</v>
       </c>
       <c r="D113" t="n">
-        <v>1.18</v>
+        <v>0.41</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>6.909</v>
+        <v>18.7</v>
       </c>
       <c r="D114" t="n">
-        <v>0.95</v>
+        <v>0.64</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3071,90 +3071,90 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>6.776</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D115" t="n">
-        <v>0.73</v>
+        <v>1.04</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>6.612</v>
+        <v>0.96</v>
       </c>
       <c r="D116" t="n">
-        <v>1.47</v>
+        <v>0.74</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6.325</v>
+        <v>7.513</v>
       </c>
       <c r="D117" t="n">
-        <v>0.99</v>
+        <v>0.85</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6.231</v>
+        <v>14.573</v>
       </c>
       <c r="D118" t="n">
-        <v>0.24</v>
+        <v>1.78</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3163,21 +3163,21 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D119" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3186,21 +3186,21 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D120" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -3209,21 +3209,21 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D121" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3232,21 +3232,21 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3255,21 +3255,21 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3278,21 +3278,21 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3301,21 +3301,21 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3324,21 +3324,21 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3347,21 +3347,21 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D127" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3370,21 +3370,21 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D128" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3393,21 +3393,21 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D129" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3416,21 +3416,21 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D130" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3439,35 +3439,334 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D131" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D143" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
+      <c r="B145" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C132" t="n">
+      <c r="C145" t="n">
         <v>6.167</v>
       </c>
-      <c r="D132" t="n">
+      <c r="D145" t="n">
         <v>0</v>
       </c>
-      <c r="E132" t="inlineStr">
+      <c r="E145" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-20 07:15
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -472,21 +472,21 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.72</v>
+        <v>3.62</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -495,21 +495,21 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17.782</v>
+        <v>18.091</v>
       </c>
       <c r="D3" t="n">
-        <v>1.5</v>
+        <v>1.74</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -518,21 +518,21 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18.7</v>
+        <v>18.721</v>
       </c>
       <c r="D4" t="n">
-        <v>0.64</v>
+        <v>0.11</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -541,21 +541,21 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3.593</v>
+        <v>3.641</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7</v>
+        <v>1.34</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -564,21 +564,21 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6.187</v>
+        <v>6.307</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03</v>
+        <v>1.94</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -587,21 +587,21 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.972</v>
+        <v>0.986</v>
       </c>
       <c r="D7" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -610,21 +610,21 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.086</v>
+        <v>1.11</v>
       </c>
       <c r="D8" t="n">
-        <v>0.93</v>
+        <v>2.21</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.72</v>
+        <v>2.763</v>
       </c>
       <c r="D9" t="n">
-        <v>0.74</v>
+        <v>1.58</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.25</v>
+        <v>8.35</v>
       </c>
       <c r="D10" t="n">
-        <v>2.17</v>
+        <v>1.21</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.923</v>
+        <v>7.998</v>
       </c>
       <c r="D11" t="n">
-        <v>4.68</v>
+        <v>0.95</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>17.909</v>
+        <v>18.455</v>
       </c>
       <c r="D12" t="n">
-        <v>5.01</v>
+        <v>3.05</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>24.167</v>
+        <v>24.333</v>
       </c>
       <c r="D13" t="n">
-        <v>1.4</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10.343</v>
+        <v>10.457</v>
       </c>
       <c r="D14" t="n">
-        <v>5.69</v>
+        <v>1.1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -831,7 +831,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -877,7 +877,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -900,7 +900,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -923,7 +923,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -946,7 +946,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D28" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1100,14 +1100,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,111 +1130,111 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D31" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>8.25</v>
+        <v>18.7</v>
       </c>
       <c r="D32" t="n">
-        <v>2.17</v>
+        <v>0.64</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.72</v>
+        <v>3.593</v>
       </c>
       <c r="D33" t="n">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D34" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D35" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1245,19 +1245,19 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1268,53 +1268,53 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.972</v>
+        <v>2.72</v>
       </c>
       <c r="D37" t="n">
-        <v>1.25</v>
+        <v>0.74</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>17.909</v>
+        <v>8.25</v>
       </c>
       <c r="D38" t="n">
-        <v>5.01</v>
+        <v>2.17</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,79 +1323,79 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D39" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.086</v>
+        <v>17.909</v>
       </c>
       <c r="D40" t="n">
-        <v>0.93</v>
+        <v>5.01</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>23.833</v>
+        <v>8.25</v>
       </c>
       <c r="D41" t="n">
-        <v>1.42</v>
+        <v>2.17</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>17.782</v>
+        <v>138</v>
       </c>
       <c r="D42" t="n">
-        <v>1.5</v>
+        <v>-0.72</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1415,148 +1415,148 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>9.715</v>
+        <v>10.343</v>
       </c>
       <c r="D43" t="n">
-        <v>3.72</v>
+        <v>5.69</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>8.074999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="D44" t="n">
-        <v>1.57</v>
+        <v>0.74</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2.7</v>
+        <v>17.782</v>
       </c>
       <c r="D45" t="n">
-        <v>1.89</v>
+        <v>1.5</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.086</v>
+        <v>24.167</v>
       </c>
       <c r="D46" t="n">
-        <v>0.93</v>
+        <v>1.4</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7.522</v>
+        <v>18.7</v>
       </c>
       <c r="D47" t="n">
-        <v>4.2</v>
+        <v>0.64</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>17.055</v>
+        <v>3.593</v>
       </c>
       <c r="D48" t="n">
-        <v>3.36</v>
+        <v>0.7</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.972</v>
+        <v>6.187</v>
       </c>
       <c r="D49" t="n">
-        <v>1.25</v>
+        <v>0.03</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1567,19 +1567,19 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6.187</v>
+        <v>0.972</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03</v>
+        <v>1.25</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1590,168 +1590,168 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.593</v>
+        <v>17.909</v>
       </c>
       <c r="D51" t="n">
-        <v>0.7</v>
+        <v>5.01</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>18.7</v>
+        <v>7.946</v>
       </c>
       <c r="D52" t="n">
-        <v>0.64</v>
+        <v>4.98</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>138</v>
+        <v>1.086</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.72</v>
+        <v>0.93</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.086</v>
+        <v>7.522</v>
       </c>
       <c r="D54" t="n">
-        <v>0.93</v>
+        <v>4.2</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>138</v>
+        <v>17.055</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.72</v>
+        <v>3.36</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>18.7</v>
+        <v>23.833</v>
       </c>
       <c r="D56" t="n">
-        <v>0.64</v>
+        <v>1.42</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>23.5</v>
+        <v>17.782</v>
       </c>
       <c r="D57" t="n">
-        <v>3.68</v>
+        <v>1.5</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1760,148 +1760,148 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>9.433</v>
+        <v>9.715</v>
       </c>
       <c r="D58" t="n">
-        <v>4.81</v>
+        <v>3.72</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>17.782</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D59" t="n">
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>7.219</v>
+        <v>2.7</v>
       </c>
       <c r="D60" t="n">
-        <v>2.27</v>
+        <v>1.89</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>7.95</v>
+        <v>138</v>
       </c>
       <c r="D61" t="n">
-        <v>2.25</v>
+        <v>-0.72</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.65</v>
+        <v>18.7</v>
       </c>
       <c r="D62" t="n">
-        <v>1.42</v>
+        <v>0.64</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>16.5</v>
+        <v>3.593</v>
       </c>
       <c r="D63" t="n">
-        <v>3.66</v>
+        <v>0.7</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.972</v>
+        <v>6.187</v>
       </c>
       <c r="D64" t="n">
-        <v>1.25</v>
+        <v>0.03</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1912,19 +1912,19 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D65" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -1935,19 +1935,19 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D66" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -1958,53 +1958,53 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>22.667</v>
+        <v>2.65</v>
       </c>
       <c r="D67" t="n">
-        <v>1.04</v>
+        <v>1.42</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.086</v>
+        <v>138</v>
       </c>
       <c r="D68" t="n">
-        <v>0.93</v>
+        <v>-0.72</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2027,19 +2027,19 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D70" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2050,352 +2050,352 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>0.972</v>
+        <v>18.7</v>
       </c>
       <c r="D71" t="n">
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>15.918</v>
+        <v>23.5</v>
       </c>
       <c r="D72" t="n">
-        <v>1.8</v>
+        <v>3.68</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2.613</v>
+        <v>9.433</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5</v>
+        <v>4.81</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>9</v>
+        <v>17.782</v>
       </c>
       <c r="D74" t="n">
         <v>1.5</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>138</v>
+        <v>7.219</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.72</v>
+        <v>2.27</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>7.059</v>
+        <v>7.95</v>
       </c>
       <c r="D76" t="n">
-        <v>0.79</v>
+        <v>2.25</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>7.775</v>
+        <v>16.5</v>
       </c>
       <c r="D77" t="n">
-        <v>0.65</v>
+        <v>3.66</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>17.782</v>
+        <v>0.972</v>
       </c>
       <c r="D78" t="n">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D79" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>18.7</v>
+        <v>1.086</v>
       </c>
       <c r="D80" t="n">
-        <v>0.64</v>
+        <v>0.93</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>22.433</v>
+        <v>3.593</v>
       </c>
       <c r="D81" t="n">
-        <v>3.14</v>
+        <v>0.7</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.972</v>
+        <v>18.7</v>
       </c>
       <c r="D82" t="n">
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>7.004</v>
+        <v>17.782</v>
       </c>
       <c r="D83" t="n">
-        <v>2.16</v>
+        <v>1.5</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>8.867000000000001</v>
+        <v>7.775</v>
       </c>
       <c r="D84" t="n">
-        <v>3.38</v>
+        <v>0.65</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>15.636</v>
+        <v>7.059</v>
       </c>
       <c r="D85" t="n">
-        <v>2.75</v>
+        <v>0.79</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2418,88 +2418,88 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>17.782</v>
+        <v>9</v>
       </c>
       <c r="D87" t="n">
         <v>1.5</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3.593</v>
+        <v>2.613</v>
       </c>
       <c r="D88" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>6.187</v>
+        <v>15.918</v>
       </c>
       <c r="D89" t="n">
-        <v>0.03</v>
+        <v>1.8</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.086</v>
+        <v>0.972</v>
       </c>
       <c r="D90" t="n">
-        <v>0.93</v>
+        <v>1.25</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2510,375 +2510,375 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2.6</v>
+        <v>6.187</v>
       </c>
       <c r="D91" t="n">
-        <v>0.97</v>
+        <v>0.03</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>7.725</v>
+        <v>22.667</v>
       </c>
       <c r="D92" t="n">
-        <v>0.8100000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>138</v>
+        <v>3.593</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.96</v>
+        <v>18.7</v>
       </c>
       <c r="D94" t="n">
-        <v>0.74</v>
+        <v>0.64</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>18.7</v>
+        <v>22.433</v>
       </c>
       <c r="D95" t="n">
-        <v>0.64</v>
+        <v>3.14</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>6.856</v>
+        <v>0.972</v>
       </c>
       <c r="D96" t="n">
-        <v>1.57</v>
+        <v>1.25</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>15.218</v>
+        <v>7.004</v>
       </c>
       <c r="D97" t="n">
-        <v>1.7</v>
+        <v>2.16</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>17.782</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D98" t="n">
-        <v>1.5</v>
+        <v>3.38</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>21.75</v>
+        <v>15.636</v>
       </c>
       <c r="D99" t="n">
-        <v>1.52</v>
+        <v>2.75</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>3.568</v>
+        <v>138</v>
       </c>
       <c r="D100" t="n">
-        <v>0.68</v>
+        <v>-0.72</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D101" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1.076</v>
+        <v>6.187</v>
       </c>
       <c r="D102" t="n">
-        <v>1.41</v>
+        <v>0.03</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>8.577</v>
+        <v>1.086</v>
       </c>
       <c r="D103" t="n">
-        <v>1.23</v>
+        <v>0.93</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>7.663</v>
+        <v>2.6</v>
       </c>
       <c r="D104" t="n">
-        <v>0.5</v>
+        <v>0.97</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>2.575</v>
+        <v>7.725</v>
       </c>
       <c r="D105" t="n">
-        <v>2.47</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>21.188</v>
+        <v>18.7</v>
       </c>
       <c r="D106" t="n">
-        <v>0.71</v>
+        <v>0.64</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2901,122 +2901,122 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>2.475</v>
+        <v>0.96</v>
       </c>
       <c r="D108" t="n">
-        <v>1.02</v>
+        <v>0.74</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D109" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>17.782</v>
+        <v>7.663</v>
       </c>
       <c r="D110" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1.076</v>
+        <v>8.577</v>
       </c>
       <c r="D111" t="n">
-        <v>1.41</v>
+        <v>1.23</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>6.584</v>
+        <v>1.076</v>
       </c>
       <c r="D112" t="n">
-        <v>0.61</v>
+        <v>1.41</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -3039,306 +3039,306 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>18.7</v>
+        <v>3.568</v>
       </c>
       <c r="D114" t="n">
-        <v>0.64</v>
+        <v>0.68</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>8.327999999999999</v>
+        <v>21.75</v>
       </c>
       <c r="D115" t="n">
-        <v>1.04</v>
+        <v>1.52</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.96</v>
+        <v>17.782</v>
       </c>
       <c r="D116" t="n">
-        <v>0.74</v>
+        <v>1.5</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>7.513</v>
+        <v>15.218</v>
       </c>
       <c r="D117" t="n">
-        <v>0.85</v>
+        <v>1.7</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>14.573</v>
+        <v>6.856</v>
       </c>
       <c r="D118" t="n">
-        <v>1.78</v>
+        <v>1.57</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>7.949</v>
+        <v>3.568</v>
       </c>
       <c r="D119" t="n">
-        <v>0.9</v>
+        <v>0.68</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>7.816</v>
+        <v>138</v>
       </c>
       <c r="D120" t="n">
-        <v>1.82</v>
+        <v>-0.72</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>7.573</v>
+        <v>17.782</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>7.535</v>
+        <v>2.475</v>
       </c>
       <c r="D122" t="n">
-        <v>0.8</v>
+        <v>1.02</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>7.475</v>
+        <v>21.188</v>
       </c>
       <c r="D123" t="n">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>7.349</v>
+        <v>14.573</v>
       </c>
       <c r="D124" t="n">
-        <v>2.21</v>
+        <v>1.78</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>7.109</v>
+        <v>7.513</v>
       </c>
       <c r="D125" t="n">
-        <v>1.43</v>
+        <v>0.85</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>7.009</v>
+        <v>0.96</v>
       </c>
       <c r="D126" t="n">
-        <v>1.18</v>
+        <v>0.74</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3347,113 +3347,113 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>6.909</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D127" t="n">
-        <v>0.95</v>
+        <v>1.04</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D128" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6.612</v>
+        <v>6.185</v>
       </c>
       <c r="D129" t="n">
-        <v>1.47</v>
+        <v>0.41</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D130" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>6.231</v>
+        <v>1.076</v>
       </c>
       <c r="D131" t="n">
-        <v>0.24</v>
+        <v>1.41</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3462,21 +3462,21 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D132" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3485,21 +3485,21 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D133" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3508,21 +3508,21 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D134" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3531,21 +3531,21 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3554,21 +3554,21 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3577,21 +3577,21 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3600,21 +3600,21 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3623,21 +3623,21 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3646,21 +3646,21 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D140" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3669,21 +3669,21 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D141" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3692,21 +3692,21 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D142" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3715,21 +3715,21 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D143" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3738,35 +3738,334 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D144" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D145" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D150" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D152" t="n">
+        <v>0</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D153" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D156" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
+      <c r="B158" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C145" t="n">
+      <c r="C158" t="n">
         <v>6.167</v>
       </c>
-      <c r="D145" t="n">
+      <c r="D158" t="n">
         <v>0</v>
       </c>
-      <c r="E145" t="inlineStr">
+      <c r="E158" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-21 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E158"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.763</v>
+        <v>2.813</v>
       </c>
       <c r="D9" t="n">
-        <v>1.58</v>
+        <v>1.81</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -659,18 +659,18 @@
         <v>8.35</v>
       </c>
       <c r="D10" t="n">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.998</v>
+        <v>7.931</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>0.09</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>18.455</v>
+        <v>18.63</v>
       </c>
       <c r="D12" t="n">
-        <v>3.05</v>
+        <v>1.8</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -728,18 +728,18 @@
         <v>24.333</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10.457</v>
+        <v>10.686</v>
       </c>
       <c r="D14" t="n">
-        <v>1.1</v>
+        <v>2.19</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -771,21 +771,21 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>17.782</v>
+        <v>18.091</v>
       </c>
       <c r="D15" t="n">
-        <v>1.5</v>
+        <v>1.74</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -794,21 +794,21 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.72</v>
+        <v>3.62</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10.343</v>
+        <v>10.457</v>
       </c>
       <c r="D17" t="n">
-        <v>5.69</v>
+        <v>1.1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>24.167</v>
+        <v>24.333</v>
       </c>
       <c r="D18" t="n">
-        <v>1.4</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17.909</v>
+        <v>18.455</v>
       </c>
       <c r="D19" t="n">
-        <v>5.01</v>
+        <v>3.05</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.923</v>
+        <v>7.998</v>
       </c>
       <c r="D20" t="n">
-        <v>4.68</v>
+        <v>0.95</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.25</v>
+        <v>8.35</v>
       </c>
       <c r="D21" t="n">
-        <v>2.17</v>
+        <v>1.21</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.72</v>
+        <v>2.763</v>
       </c>
       <c r="D22" t="n">
-        <v>0.74</v>
+        <v>1.58</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -955,21 +955,21 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.086</v>
+        <v>1.11</v>
       </c>
       <c r="D23" t="n">
-        <v>0.93</v>
+        <v>2.21</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -978,21 +978,21 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.972</v>
+        <v>0.986</v>
       </c>
       <c r="D24" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1001,21 +1001,21 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6.187</v>
+        <v>6.307</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03</v>
+        <v>1.94</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1024,21 +1024,21 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.593</v>
+        <v>3.641</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7</v>
+        <v>1.34</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1047,44 +1047,44 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>18.7</v>
+        <v>18.721</v>
       </c>
       <c r="D27" t="n">
-        <v>0.64</v>
+        <v>0.11</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D28" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1107,7 +1107,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,30 +1130,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D31" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1176,7 +1176,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1199,7 +1199,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1291,7 +1291,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1314,7 +1314,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1337,7 +1337,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1360,30 +1360,30 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>8.25</v>
+        <v>18.7</v>
       </c>
       <c r="D41" t="n">
-        <v>2.17</v>
+        <v>0.64</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1406,76 +1406,76 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D43" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>2.72</v>
+        <v>3.593</v>
       </c>
       <c r="D44" t="n">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D45" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1491,49 +1491,49 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D47" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D48" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1544,19 +1544,19 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1567,53 +1567,53 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.972</v>
+        <v>2.72</v>
       </c>
       <c r="D50" t="n">
-        <v>1.25</v>
+        <v>0.74</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>17.909</v>
+        <v>8.25</v>
       </c>
       <c r="D51" t="n">
-        <v>5.01</v>
+        <v>2.17</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1622,125 +1622,125 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D52" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.086</v>
+        <v>17.909</v>
       </c>
       <c r="D53" t="n">
-        <v>0.93</v>
+        <v>5.01</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>7.522</v>
+        <v>18.7</v>
       </c>
       <c r="D54" t="n">
-        <v>4.2</v>
+        <v>0.64</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>17.055</v>
+        <v>3.593</v>
       </c>
       <c r="D55" t="n">
-        <v>3.36</v>
+        <v>0.7</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>23.833</v>
+        <v>8.25</v>
       </c>
       <c r="D56" t="n">
-        <v>1.42</v>
+        <v>2.17</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>17.782</v>
+        <v>138</v>
       </c>
       <c r="D57" t="n">
-        <v>1.5</v>
+        <v>-0.72</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1760,148 +1760,148 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>9.715</v>
+        <v>10.343</v>
       </c>
       <c r="D58" t="n">
-        <v>3.72</v>
+        <v>5.69</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>8.074999999999999</v>
+        <v>2.72</v>
       </c>
       <c r="D59" t="n">
-        <v>1.57</v>
+        <v>0.74</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.7</v>
+        <v>17.782</v>
       </c>
       <c r="D60" t="n">
-        <v>1.89</v>
+        <v>1.5</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>138</v>
+        <v>1.086</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.72</v>
+        <v>0.93</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>18.7</v>
+        <v>7.946</v>
       </c>
       <c r="D62" t="n">
-        <v>0.64</v>
+        <v>4.98</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3.593</v>
+        <v>17.909</v>
       </c>
       <c r="D63" t="n">
-        <v>0.7</v>
+        <v>5.01</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.187</v>
+        <v>0.972</v>
       </c>
       <c r="D64" t="n">
-        <v>0.03</v>
+        <v>1.25</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1912,42 +1912,42 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1.086</v>
+        <v>24.167</v>
       </c>
       <c r="D65" t="n">
-        <v>0.93</v>
+        <v>1.4</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.972</v>
+        <v>6.187</v>
       </c>
       <c r="D66" t="n">
-        <v>1.25</v>
+        <v>0.03</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -1958,65 +1958,65 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.65</v>
+        <v>18.7</v>
       </c>
       <c r="D67" t="n">
-        <v>1.42</v>
+        <v>0.64</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>138</v>
+        <v>17.055</v>
       </c>
       <c r="D68" t="n">
-        <v>-0.72</v>
+        <v>3.36</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D69" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2027,76 +2027,76 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.086</v>
+        <v>7.522</v>
       </c>
       <c r="D70" t="n">
-        <v>0.93</v>
+        <v>4.2</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>18.7</v>
+        <v>23.833</v>
       </c>
       <c r="D71" t="n">
-        <v>0.64</v>
+        <v>1.42</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>23.5</v>
+        <v>17.782</v>
       </c>
       <c r="D72" t="n">
-        <v>3.68</v>
+        <v>1.5</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2105,125 +2105,125 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>9.433</v>
+        <v>9.715</v>
       </c>
       <c r="D73" t="n">
-        <v>4.81</v>
+        <v>3.72</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>17.782</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D74" t="n">
-        <v>1.5</v>
+        <v>1.57</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>7.219</v>
+        <v>2.7</v>
       </c>
       <c r="D75" t="n">
-        <v>2.27</v>
+        <v>1.89</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>7.95</v>
+        <v>138</v>
       </c>
       <c r="D76" t="n">
-        <v>2.25</v>
+        <v>-0.72</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>16.5</v>
+        <v>3.593</v>
       </c>
       <c r="D77" t="n">
-        <v>3.66</v>
+        <v>0.7</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.972</v>
+        <v>6.187</v>
       </c>
       <c r="D78" t="n">
-        <v>1.25</v>
+        <v>0.03</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2234,19 +2234,19 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D79" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2257,30 +2257,30 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.086</v>
+        <v>138</v>
       </c>
       <c r="D80" t="n">
-        <v>0.93</v>
+        <v>-0.72</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2303,226 +2303,226 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D82" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>17.782</v>
+        <v>0.972</v>
       </c>
       <c r="D83" t="n">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.775</v>
+        <v>16.5</v>
       </c>
       <c r="D84" t="n">
-        <v>0.65</v>
+        <v>3.66</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7.059</v>
+        <v>7.95</v>
       </c>
       <c r="D85" t="n">
-        <v>0.79</v>
+        <v>2.25</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>138</v>
+        <v>7.219</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.72</v>
+        <v>2.27</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>9</v>
+        <v>17.782</v>
       </c>
       <c r="D87" t="n">
         <v>1.5</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2.613</v>
+        <v>9.433</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5</v>
+        <v>4.81</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>15.918</v>
+        <v>23.5</v>
       </c>
       <c r="D89" t="n">
-        <v>1.8</v>
+        <v>3.68</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.972</v>
+        <v>18.7</v>
       </c>
       <c r="D90" t="n">
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D91" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2533,191 +2533,191 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>22.667</v>
+        <v>2.65</v>
       </c>
       <c r="D92" t="n">
-        <v>1.04</v>
+        <v>1.42</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>3.593</v>
+        <v>9</v>
       </c>
       <c r="D93" t="n">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>18.7</v>
+        <v>1.086</v>
       </c>
       <c r="D94" t="n">
-        <v>0.64</v>
+        <v>0.93</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>22.433</v>
+        <v>3.593</v>
       </c>
       <c r="D95" t="n">
-        <v>3.14</v>
+        <v>0.7</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.972</v>
+        <v>18.7</v>
       </c>
       <c r="D96" t="n">
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7.004</v>
+        <v>17.782</v>
       </c>
       <c r="D97" t="n">
-        <v>2.16</v>
+        <v>1.5</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>8.867000000000001</v>
+        <v>7.775</v>
       </c>
       <c r="D98" t="n">
-        <v>3.38</v>
+        <v>0.65</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>15.636</v>
+        <v>7.059</v>
       </c>
       <c r="D99" t="n">
-        <v>2.75</v>
+        <v>0.79</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2740,65 +2740,65 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>17.782</v>
+        <v>2.613</v>
       </c>
       <c r="D101" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>6.187</v>
+        <v>15.918</v>
       </c>
       <c r="D102" t="n">
-        <v>0.03</v>
+        <v>1.8</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.086</v>
+        <v>0.972</v>
       </c>
       <c r="D103" t="n">
-        <v>0.93</v>
+        <v>1.25</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2809,375 +2809,375 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>2.6</v>
+        <v>6.187</v>
       </c>
       <c r="D104" t="n">
-        <v>0.97</v>
+        <v>0.03</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>7.725</v>
+        <v>22.667</v>
       </c>
       <c r="D105" t="n">
-        <v>0.8100000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>18.7</v>
+        <v>3.593</v>
       </c>
       <c r="D106" t="n">
-        <v>0.64</v>
+        <v>0.7</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>138</v>
+        <v>22.433</v>
       </c>
       <c r="D107" t="n">
-        <v>-0.72</v>
+        <v>3.14</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.96</v>
+        <v>18.7</v>
       </c>
       <c r="D108" t="n">
-        <v>0.74</v>
+        <v>0.64</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>2.575</v>
+        <v>7.725</v>
       </c>
       <c r="D109" t="n">
-        <v>2.47</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>7.663</v>
+        <v>2.6</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5</v>
+        <v>0.97</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>8.577</v>
+        <v>1.086</v>
       </c>
       <c r="D111" t="n">
-        <v>1.23</v>
+        <v>0.93</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1.076</v>
+        <v>6.187</v>
       </c>
       <c r="D112" t="n">
-        <v>1.41</v>
+        <v>0.03</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D113" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>3.568</v>
+        <v>138</v>
       </c>
       <c r="D114" t="n">
-        <v>0.68</v>
+        <v>-0.72</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>21.75</v>
+        <v>15.636</v>
       </c>
       <c r="D115" t="n">
-        <v>1.52</v>
+        <v>2.75</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>17.782</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D116" t="n">
-        <v>1.5</v>
+        <v>3.38</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>15.218</v>
+        <v>7.004</v>
       </c>
       <c r="D117" t="n">
-        <v>1.7</v>
+        <v>2.16</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>6.856</v>
+        <v>0.972</v>
       </c>
       <c r="D118" t="n">
-        <v>1.57</v>
+        <v>1.25</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>3.568</v>
+        <v>2.575</v>
       </c>
       <c r="D119" t="n">
-        <v>0.68</v>
+        <v>2.47</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3200,134 +3200,134 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>17.782</v>
+        <v>7.663</v>
       </c>
       <c r="D121" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2.475</v>
+        <v>0.96</v>
       </c>
       <c r="D122" t="n">
-        <v>1.02</v>
+        <v>0.74</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>21.188</v>
+        <v>18.7</v>
       </c>
       <c r="D123" t="n">
-        <v>0.71</v>
+        <v>0.64</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>14.573</v>
+        <v>8.577</v>
       </c>
       <c r="D124" t="n">
-        <v>1.78</v>
+        <v>1.23</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>7.513</v>
+        <v>1.076</v>
       </c>
       <c r="D125" t="n">
-        <v>0.85</v>
+        <v>1.41</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.96</v>
+        <v>6.185</v>
       </c>
       <c r="D126" t="n">
-        <v>0.74</v>
+        <v>0.41</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3338,398 +3338,398 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>8.327999999999999</v>
+        <v>3.568</v>
       </c>
       <c r="D127" t="n">
-        <v>1.04</v>
+        <v>0.68</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>18.7</v>
+        <v>21.75</v>
       </c>
       <c r="D128" t="n">
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6.185</v>
+        <v>17.782</v>
       </c>
       <c r="D129" t="n">
-        <v>0.41</v>
+        <v>1.5</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>6.584</v>
+        <v>15.218</v>
       </c>
       <c r="D130" t="n">
-        <v>0.61</v>
+        <v>1.7</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1.076</v>
+        <v>6.856</v>
       </c>
       <c r="D131" t="n">
-        <v>1.41</v>
+        <v>1.57</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>7.949</v>
+        <v>14.573</v>
       </c>
       <c r="D132" t="n">
-        <v>0.9</v>
+        <v>1.78</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>7.816</v>
+        <v>7.513</v>
       </c>
       <c r="D133" t="n">
-        <v>1.82</v>
+        <v>0.85</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>7.573</v>
+        <v>3.568</v>
       </c>
       <c r="D134" t="n">
-        <v>0.5</v>
+        <v>0.68</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7.535</v>
+        <v>138</v>
       </c>
       <c r="D135" t="n">
-        <v>0.8</v>
+        <v>-0.72</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>7.475</v>
+        <v>17.782</v>
       </c>
       <c r="D136" t="n">
-        <v>0.86</v>
+        <v>1.5</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7.349</v>
+        <v>2.475</v>
       </c>
       <c r="D137" t="n">
-        <v>2.21</v>
+        <v>1.02</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>7.109</v>
+        <v>1.076</v>
       </c>
       <c r="D138" t="n">
-        <v>1.43</v>
+        <v>1.41</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>7.009</v>
+        <v>6.584</v>
       </c>
       <c r="D139" t="n">
-        <v>1.18</v>
+        <v>0.61</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6.909</v>
+        <v>6.185</v>
       </c>
       <c r="D140" t="n">
-        <v>0.95</v>
+        <v>0.41</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D141" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>6.612</v>
+        <v>21.188</v>
       </c>
       <c r="D142" t="n">
-        <v>1.47</v>
+        <v>0.71</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6.325</v>
+        <v>0.96</v>
       </c>
       <c r="D143" t="n">
-        <v>0.99</v>
+        <v>0.74</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3738,21 +3738,21 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>6.231</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D144" t="n">
-        <v>0.24</v>
+        <v>1.04</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -3761,21 +3761,21 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D145" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3784,21 +3784,21 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D146" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -3807,21 +3807,21 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D147" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -3830,21 +3830,21 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -3853,21 +3853,21 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -3876,21 +3876,21 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3899,21 +3899,21 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3922,21 +3922,21 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -3945,21 +3945,21 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D153" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -3968,21 +3968,21 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D154" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -3991,21 +3991,21 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D155" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -4014,21 +4014,21 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D156" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -4037,35 +4037,334 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D157" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D160" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D162" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D163" t="n">
+        <v>0</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D164" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D165" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D166" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D167" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D168" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D169" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D170" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
+      <c r="B171" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C158" t="n">
+      <c r="C171" t="n">
         <v>6.167</v>
       </c>
-      <c r="D158" t="n">
+      <c r="D171" t="n">
         <v>0</v>
       </c>
-      <c r="E158" t="inlineStr">
+      <c r="E171" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-22 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.813</v>
+        <v>2.893</v>
       </c>
       <c r="D9" t="n">
-        <v>1.81</v>
+        <v>2.84</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.35</v>
+        <v>8.363</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.931</v>
+        <v>8.069000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>0.09</v>
+        <v>1.74</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>18.63</v>
+        <v>19.25</v>
       </c>
       <c r="D12" t="n">
-        <v>1.8</v>
+        <v>3.33</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>24.333</v>
+        <v>24.368</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10.686</v>
+        <v>11.267</v>
       </c>
       <c r="D14" t="n">
-        <v>2.19</v>
+        <v>4.88</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10.457</v>
+        <v>10.686</v>
       </c>
       <c r="D17" t="n">
-        <v>1.1</v>
+        <v>2.19</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -843,18 +843,18 @@
         <v>24.333</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>18.455</v>
+        <v>18.63</v>
       </c>
       <c r="D19" t="n">
-        <v>3.05</v>
+        <v>1.8</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.998</v>
+        <v>7.931</v>
       </c>
       <c r="D20" t="n">
-        <v>0.95</v>
+        <v>0.09</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -912,18 +912,18 @@
         <v>8.35</v>
       </c>
       <c r="D21" t="n">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.763</v>
+        <v>2.813</v>
       </c>
       <c r="D22" t="n">
-        <v>1.58</v>
+        <v>1.81</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>10.343</v>
+        <v>18.091</v>
       </c>
       <c r="D28" t="n">
-        <v>5.69</v>
+        <v>1.74</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1093,21 +1093,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>24.167</v>
+        <v>24.333</v>
       </c>
       <c r="D29" t="n">
-        <v>1.4</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1116,44 +1116,44 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.72</v>
+        <v>3.62</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>17.782</v>
+        <v>10.457</v>
       </c>
       <c r="D31" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1162,21 +1162,21 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>18.7</v>
+        <v>18.721</v>
       </c>
       <c r="D32" t="n">
-        <v>0.64</v>
+        <v>0.11</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1185,21 +1185,21 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.593</v>
+        <v>3.641</v>
       </c>
       <c r="D33" t="n">
-        <v>0.7</v>
+        <v>1.34</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1208,21 +1208,21 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6.187</v>
+        <v>6.307</v>
       </c>
       <c r="D34" t="n">
-        <v>0.03</v>
+        <v>1.94</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1231,21 +1231,21 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.972</v>
+        <v>0.986</v>
       </c>
       <c r="D35" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1254,21 +1254,21 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1.086</v>
+        <v>1.11</v>
       </c>
       <c r="D36" t="n">
-        <v>0.93</v>
+        <v>2.21</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1277,21 +1277,21 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.72</v>
+        <v>2.763</v>
       </c>
       <c r="D37" t="n">
-        <v>0.74</v>
+        <v>1.58</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1300,21 +1300,21 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>8.25</v>
+        <v>8.35</v>
       </c>
       <c r="D38" t="n">
-        <v>2.17</v>
+        <v>1.21</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,21 +1323,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.923</v>
+        <v>7.998</v>
       </c>
       <c r="D39" t="n">
-        <v>4.68</v>
+        <v>0.95</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1346,21 +1346,21 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>17.909</v>
+        <v>18.455</v>
       </c>
       <c r="D40" t="n">
-        <v>5.01</v>
+        <v>3.05</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1383,122 +1383,122 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>138</v>
+        <v>3.593</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>17.782</v>
+        <v>24.167</v>
       </c>
       <c r="D43" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.593</v>
+        <v>10.343</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7</v>
+        <v>5.69</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D45" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>24.167</v>
+        <v>138</v>
       </c>
       <c r="D46" t="n">
-        <v>1.4</v>
+        <v>-0.72</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1521,7 +1521,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1544,7 +1544,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1567,7 +1567,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1590,7 +1590,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1613,7 +1613,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1659,42 +1659,42 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D54" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D55" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1705,30 +1705,30 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>8.25</v>
+        <v>18.7</v>
       </c>
       <c r="D56" t="n">
-        <v>2.17</v>
+        <v>0.64</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1751,99 +1751,99 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D58" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.72</v>
+        <v>3.593</v>
       </c>
       <c r="D59" t="n">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D60" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1.086</v>
+        <v>17.909</v>
       </c>
       <c r="D61" t="n">
-        <v>0.93</v>
+        <v>5.01</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1852,67 +1852,67 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D62" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>17.909</v>
+        <v>8.25</v>
       </c>
       <c r="D63" t="n">
-        <v>5.01</v>
+        <v>2.17</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.972</v>
+        <v>2.72</v>
       </c>
       <c r="D64" t="n">
-        <v>1.25</v>
+        <v>0.74</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1928,26 +1928,26 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D66" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -1958,65 +1958,65 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>18.7</v>
+        <v>1.086</v>
       </c>
       <c r="D67" t="n">
-        <v>0.64</v>
+        <v>0.93</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>17.055</v>
+        <v>18.7</v>
       </c>
       <c r="D68" t="n">
-        <v>3.36</v>
+        <v>0.64</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.972</v>
+        <v>3.593</v>
       </c>
       <c r="D69" t="n">
-        <v>1.25</v>
+        <v>0.7</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2027,180 +2027,180 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>7.522</v>
+        <v>8.25</v>
       </c>
       <c r="D70" t="n">
-        <v>4.2</v>
+        <v>2.17</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>23.833</v>
+        <v>138</v>
       </c>
       <c r="D71" t="n">
-        <v>1.42</v>
+        <v>-0.72</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D72" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>9.715</v>
+        <v>2.72</v>
       </c>
       <c r="D73" t="n">
-        <v>3.72</v>
+        <v>0.74</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>8.074999999999999</v>
+        <v>17.782</v>
       </c>
       <c r="D74" t="n">
-        <v>1.57</v>
+        <v>1.5</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2.7</v>
+        <v>7.946</v>
       </c>
       <c r="D75" t="n">
-        <v>1.89</v>
+        <v>4.98</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>138</v>
+        <v>17.909</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.72</v>
+        <v>5.01</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D77" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2211,42 +2211,42 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.187</v>
+        <v>24.167</v>
       </c>
       <c r="D78" t="n">
-        <v>0.03</v>
+        <v>1.4</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.086</v>
+        <v>6.187</v>
       </c>
       <c r="D79" t="n">
-        <v>0.93</v>
+        <v>0.03</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2257,65 +2257,65 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>138</v>
+        <v>17.055</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.72</v>
+        <v>3.36</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>3.593</v>
+        <v>18.7</v>
       </c>
       <c r="D81" t="n">
-        <v>0.7</v>
+        <v>0.64</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>6.187</v>
+        <v>0.972</v>
       </c>
       <c r="D82" t="n">
-        <v>0.03</v>
+        <v>1.25</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2326,19 +2326,19 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.972</v>
+        <v>1.086</v>
       </c>
       <c r="D83" t="n">
-        <v>1.25</v>
+        <v>0.93</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2349,157 +2349,157 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>16.5</v>
+        <v>7.522</v>
       </c>
       <c r="D84" t="n">
-        <v>3.66</v>
+        <v>4.2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7.95</v>
+        <v>23.833</v>
       </c>
       <c r="D85" t="n">
-        <v>2.25</v>
+        <v>1.42</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7.219</v>
+        <v>17.782</v>
       </c>
       <c r="D86" t="n">
-        <v>2.27</v>
+        <v>1.5</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>17.782</v>
+        <v>9.715</v>
       </c>
       <c r="D87" t="n">
-        <v>1.5</v>
+        <v>3.72</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>9.433</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D88" t="n">
-        <v>4.81</v>
+        <v>1.57</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>23.5</v>
+        <v>2.7</v>
       </c>
       <c r="D89" t="n">
-        <v>3.68</v>
+        <v>1.89</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>18.7</v>
+        <v>138</v>
       </c>
       <c r="D90" t="n">
-        <v>0.64</v>
+        <v>-0.72</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2510,19 +2510,19 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1.086</v>
+        <v>3.593</v>
       </c>
       <c r="D91" t="n">
-        <v>0.93</v>
+        <v>0.7</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2533,513 +2533,513 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.65</v>
+        <v>6.187</v>
       </c>
       <c r="D92" t="n">
-        <v>1.42</v>
+        <v>0.03</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>9</v>
+        <v>0.972</v>
       </c>
       <c r="D93" t="n">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.086</v>
+        <v>138</v>
       </c>
       <c r="D94" t="n">
-        <v>0.93</v>
+        <v>-0.72</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>3.593</v>
+        <v>16.5</v>
       </c>
       <c r="D95" t="n">
-        <v>0.7</v>
+        <v>3.66</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>18.7</v>
+        <v>3.593</v>
       </c>
       <c r="D96" t="n">
-        <v>0.64</v>
+        <v>0.7</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>17.782</v>
+        <v>2.65</v>
       </c>
       <c r="D97" t="n">
-        <v>1.5</v>
+        <v>1.42</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7.775</v>
+        <v>1.086</v>
       </c>
       <c r="D98" t="n">
-        <v>0.65</v>
+        <v>0.93</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>7.059</v>
+        <v>18.7</v>
       </c>
       <c r="D99" t="n">
-        <v>0.79</v>
+        <v>0.64</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>138</v>
+        <v>23.5</v>
       </c>
       <c r="D100" t="n">
-        <v>-0.72</v>
+        <v>3.68</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2.613</v>
+        <v>9.433</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5</v>
+        <v>4.81</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>15.918</v>
+        <v>6.187</v>
       </c>
       <c r="D102" t="n">
-        <v>1.8</v>
+        <v>0.03</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.972</v>
+        <v>7.219</v>
       </c>
       <c r="D103" t="n">
-        <v>1.25</v>
+        <v>2.27</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6.187</v>
+        <v>7.95</v>
       </c>
       <c r="D104" t="n">
-        <v>0.03</v>
+        <v>2.25</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>22.667</v>
+        <v>17.782</v>
       </c>
       <c r="D105" t="n">
-        <v>1.04</v>
+        <v>1.5</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>3.593</v>
+        <v>2.613</v>
       </c>
       <c r="D106" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>22.433</v>
+        <v>9</v>
       </c>
       <c r="D107" t="n">
-        <v>3.14</v>
+        <v>1.5</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>18.7</v>
+        <v>1.086</v>
       </c>
       <c r="D108" t="n">
-        <v>0.64</v>
+        <v>0.93</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>7.725</v>
+        <v>3.593</v>
       </c>
       <c r="D109" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>2.6</v>
+        <v>18.7</v>
       </c>
       <c r="D110" t="n">
-        <v>0.97</v>
+        <v>0.64</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1.086</v>
+        <v>17.782</v>
       </c>
       <c r="D111" t="n">
-        <v>0.93</v>
+        <v>1.5</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>6.187</v>
+        <v>7.775</v>
       </c>
       <c r="D112" t="n">
-        <v>0.03</v>
+        <v>0.65</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>17.782</v>
+        <v>7.059</v>
       </c>
       <c r="D113" t="n">
-        <v>1.5</v>
+        <v>0.79</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -3062,7 +3062,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3071,159 +3071,159 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15.636</v>
+        <v>15.918</v>
       </c>
       <c r="D115" t="n">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>8.867000000000001</v>
+        <v>0.972</v>
       </c>
       <c r="D116" t="n">
-        <v>3.38</v>
+        <v>1.25</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>7.004</v>
+        <v>6.187</v>
       </c>
       <c r="D117" t="n">
-        <v>2.16</v>
+        <v>0.03</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.972</v>
+        <v>22.667</v>
       </c>
       <c r="D118" t="n">
-        <v>1.25</v>
+        <v>1.04</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>2.575</v>
+        <v>18.7</v>
       </c>
       <c r="D119" t="n">
-        <v>2.47</v>
+        <v>0.64</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>138</v>
+        <v>3.593</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>7.663</v>
+        <v>22.433</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5</v>
+        <v>3.14</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3232,44 +3232,44 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D122" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>18.7</v>
+        <v>7.004</v>
       </c>
       <c r="D123" t="n">
-        <v>0.64</v>
+        <v>2.16</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3278,320 +3278,320 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>8.577</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D124" t="n">
-        <v>1.23</v>
+        <v>3.38</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1.076</v>
+        <v>15.636</v>
       </c>
       <c r="D125" t="n">
-        <v>1.41</v>
+        <v>2.75</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>6.185</v>
+        <v>138</v>
       </c>
       <c r="D126" t="n">
-        <v>0.41</v>
+        <v>-0.72</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>3.568</v>
+        <v>17.782</v>
       </c>
       <c r="D127" t="n">
-        <v>0.68</v>
+        <v>1.5</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>21.75</v>
+        <v>6.187</v>
       </c>
       <c r="D128" t="n">
-        <v>1.52</v>
+        <v>0.03</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>17.782</v>
+        <v>1.086</v>
       </c>
       <c r="D129" t="n">
-        <v>1.5</v>
+        <v>0.93</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>15.218</v>
+        <v>2.6</v>
       </c>
       <c r="D130" t="n">
-        <v>1.7</v>
+        <v>0.97</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>6.856</v>
+        <v>7.725</v>
       </c>
       <c r="D131" t="n">
-        <v>1.57</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>14.573</v>
+        <v>0.96</v>
       </c>
       <c r="D132" t="n">
-        <v>1.78</v>
+        <v>0.74</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>7.513</v>
+        <v>138</v>
       </c>
       <c r="D133" t="n">
-        <v>0.85</v>
+        <v>-0.72</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>3.568</v>
+        <v>18.7</v>
       </c>
       <c r="D134" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>138</v>
+        <v>7.663</v>
       </c>
       <c r="D135" t="n">
-        <v>-0.72</v>
+        <v>0.5</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>17.782</v>
+        <v>2.575</v>
       </c>
       <c r="D136" t="n">
-        <v>1.5</v>
+        <v>2.47</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>2.475</v>
+        <v>8.577</v>
       </c>
       <c r="D137" t="n">
-        <v>1.02</v>
+        <v>1.23</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3614,42 +3614,42 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6.584</v>
+        <v>6.185</v>
       </c>
       <c r="D139" t="n">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>6.185</v>
+        <v>3.568</v>
       </c>
       <c r="D140" t="n">
-        <v>0.41</v>
+        <v>0.68</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3660,237 +3660,237 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>18.7</v>
+        <v>21.75</v>
       </c>
       <c r="D141" t="n">
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>21.188</v>
+        <v>17.782</v>
       </c>
       <c r="D142" t="n">
-        <v>0.71</v>
+        <v>1.5</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.96</v>
+        <v>15.218</v>
       </c>
       <c r="D143" t="n">
-        <v>0.74</v>
+        <v>1.7</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>8.327999999999999</v>
+        <v>6.856</v>
       </c>
       <c r="D144" t="n">
-        <v>1.04</v>
+        <v>1.57</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>7.949</v>
+        <v>2.475</v>
       </c>
       <c r="D145" t="n">
-        <v>0.9</v>
+        <v>1.02</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>7.816</v>
+        <v>1.076</v>
       </c>
       <c r="D146" t="n">
-        <v>1.82</v>
+        <v>1.41</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>7.573</v>
+        <v>14.573</v>
       </c>
       <c r="D147" t="n">
-        <v>0.5</v>
+        <v>1.78</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7.535</v>
+        <v>7.513</v>
       </c>
       <c r="D148" t="n">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>7.475</v>
+        <v>3.568</v>
       </c>
       <c r="D149" t="n">
-        <v>0.86</v>
+        <v>0.68</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>7.349</v>
+        <v>138</v>
       </c>
       <c r="D150" t="n">
-        <v>2.21</v>
+        <v>-0.72</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3899,159 +3899,159 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>7.109</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D151" t="n">
-        <v>1.43</v>
+        <v>1.04</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>7.009</v>
+        <v>0.96</v>
       </c>
       <c r="D152" t="n">
-        <v>1.18</v>
+        <v>0.74</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>6.909</v>
+        <v>21.188</v>
       </c>
       <c r="D153" t="n">
-        <v>0.95</v>
+        <v>0.71</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D154" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>6.612</v>
+        <v>17.782</v>
       </c>
       <c r="D155" t="n">
-        <v>1.47</v>
+        <v>1.5</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D156" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>6.231</v>
+        <v>6.185</v>
       </c>
       <c r="D157" t="n">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -4060,21 +4060,21 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D158" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -4083,21 +4083,21 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D159" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4106,21 +4106,21 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D160" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -4129,21 +4129,21 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D161" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -4152,21 +4152,21 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -4175,21 +4175,21 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -4198,21 +4198,21 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4221,21 +4221,21 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -4244,21 +4244,21 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D166" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -4267,21 +4267,21 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D167" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -4290,21 +4290,21 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D168" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -4313,21 +4313,21 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D169" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4336,35 +4336,334 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D170" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D171" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D173" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D174" t="n">
+        <v>0</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D175" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D177" t="n">
+        <v>0</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D178" t="n">
+        <v>0</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D179" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D180" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D181" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D182" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D183" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
+      <c r="B184" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C171" t="n">
+      <c r="C184" t="n">
         <v>6.167</v>
       </c>
-      <c r="D171" t="n">
+      <c r="D184" t="n">
         <v>0</v>
       </c>
-      <c r="E171" t="inlineStr">
+      <c r="E184" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>

<commit_message>
Auto update: 2025-10-23 07:14
</commit_message>
<xml_diff>
--- a/DRAMeXchange_Semi_price.xlsx
+++ b/DRAMeXchange_Semi_price.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -509,7 +509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -555,7 +555,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -578,7 +578,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,7 +601,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -624,7 +624,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -633,21 +633,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2.893</v>
+        <v>2.975</v>
       </c>
       <c r="D9" t="n">
-        <v>2.84</v>
+        <v>2.83</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -656,21 +656,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>8.363</v>
+        <v>8.375</v>
       </c>
       <c r="D10" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -679,21 +679,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8.069000000000001</v>
+        <v>8.316000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>1.74</v>
+        <v>3.06</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -702,21 +702,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>19.25</v>
+        <v>19.8</v>
       </c>
       <c r="D12" t="n">
-        <v>3.33</v>
+        <v>2.86</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -725,21 +725,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>24.368</v>
+        <v>24.566</v>
       </c>
       <c r="D13" t="n">
-        <v>0.14</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -748,21 +748,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>11.267</v>
+        <v>11.867</v>
       </c>
       <c r="D14" t="n">
-        <v>4.88</v>
+        <v>5.33</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Oct.22 2025    14:40</t>
+          <t>Oct.23 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -785,7 +785,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -817,21 +817,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10.686</v>
+        <v>11.267</v>
       </c>
       <c r="D17" t="n">
-        <v>2.19</v>
+        <v>4.88</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -840,21 +840,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>24.333</v>
+        <v>24.368</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -863,21 +863,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>18.63</v>
+        <v>19.25</v>
       </c>
       <c r="D19" t="n">
-        <v>1.8</v>
+        <v>3.33</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -886,21 +886,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7.931</v>
+        <v>8.069000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>0.09</v>
+        <v>1.74</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -909,21 +909,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.35</v>
+        <v>8.363</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -932,21 +932,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.813</v>
+        <v>2.893</v>
       </c>
       <c r="D22" t="n">
-        <v>1.81</v>
+        <v>2.84</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Oct.21 2025    14:40</t>
+          <t>Oct.22 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -969,7 +969,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -992,7 +992,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1015,7 +1015,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1038,7 +1038,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1061,30 +1061,30 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>18.091</v>
+        <v>10.686</v>
       </c>
       <c r="D28" t="n">
-        <v>1.74</v>
+        <v>2.19</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oct.13 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1096,18 +1096,18 @@
         <v>24.333</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1130,30 +1130,30 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>10.457</v>
+        <v>18.091</v>
       </c>
       <c r="D31" t="n">
-        <v>1.1</v>
+        <v>1.74</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1176,7 +1176,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1199,7 +1199,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1222,7 +1222,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1245,7 +1245,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1277,21 +1277,21 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.763</v>
+        <v>2.813</v>
       </c>
       <c r="D37" t="n">
-        <v>1.58</v>
+        <v>1.81</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1303,18 +1303,18 @@
         <v>8.35</v>
       </c>
       <c r="D38" t="n">
-        <v>1.21</v>
+        <v>0</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1323,21 +1323,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7.998</v>
+        <v>7.931</v>
       </c>
       <c r="D39" t="n">
-        <v>0.95</v>
+        <v>0.09</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1346,21 +1346,21 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>18.455</v>
+        <v>18.63</v>
       </c>
       <c r="D40" t="n">
-        <v>3.05</v>
+        <v>1.8</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Oct.20 2025    14:40</t>
+          <t>Oct.21 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1369,21 +1369,21 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>18.7</v>
+        <v>18.721</v>
       </c>
       <c r="D41" t="n">
-        <v>0.64</v>
+        <v>0.11</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1392,21 +1392,21 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.593</v>
+        <v>3.641</v>
       </c>
       <c r="D42" t="n">
-        <v>0.7</v>
+        <v>1.34</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1415,67 +1415,67 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>24.167</v>
+        <v>24.333</v>
       </c>
       <c r="D43" t="n">
-        <v>1.4</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>10.343</v>
+        <v>18.091</v>
       </c>
       <c r="D44" t="n">
-        <v>5.69</v>
+        <v>1.74</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17.782</v>
+        <v>10.457</v>
       </c>
       <c r="D45" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1484,21 +1484,21 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.72</v>
+        <v>3.62</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1507,21 +1507,21 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>6.187</v>
+        <v>6.307</v>
       </c>
       <c r="D47" t="n">
-        <v>0.03</v>
+        <v>1.94</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1530,21 +1530,21 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.972</v>
+        <v>0.986</v>
       </c>
       <c r="D48" t="n">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1553,21 +1553,21 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.086</v>
+        <v>1.11</v>
       </c>
       <c r="D49" t="n">
-        <v>0.93</v>
+        <v>2.21</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.13 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1576,21 +1576,21 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.72</v>
+        <v>2.763</v>
       </c>
       <c r="D50" t="n">
-        <v>0.74</v>
+        <v>1.58</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1599,21 +1599,21 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>8.25</v>
+        <v>8.35</v>
       </c>
       <c r="D51" t="n">
-        <v>2.17</v>
+        <v>1.21</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1622,21 +1622,21 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7.923</v>
+        <v>7.998</v>
       </c>
       <c r="D52" t="n">
-        <v>4.68</v>
+        <v>0.95</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-10-19</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1645,21 +1645,21 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>17.909</v>
+        <v>18.455</v>
       </c>
       <c r="D53" t="n">
-        <v>5.01</v>
+        <v>3.05</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.20 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1682,7 +1682,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1705,7 +1705,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1728,99 +1728,99 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>138</v>
+        <v>3.593</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.72</v>
+        <v>0.7</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>17.782</v>
+        <v>24.167</v>
       </c>
       <c r="D58" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3.593</v>
+        <v>10.343</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7</v>
+        <v>5.69</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D60" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1843,7 +1843,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1866,7 +1866,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1889,7 +1889,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1912,30 +1912,30 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>24.167</v>
+        <v>138</v>
       </c>
       <c r="D65" t="n">
-        <v>1.4</v>
+        <v>-0.72</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Oct.17 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-19</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1958,65 +1958,65 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.086</v>
+        <v>17.909</v>
       </c>
       <c r="D67" t="n">
-        <v>0.93</v>
+        <v>5.01</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>18.7</v>
+        <v>6.187</v>
       </c>
       <c r="D68" t="n">
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D69" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2027,30 +2027,30 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>8.25</v>
+        <v>18.7</v>
       </c>
       <c r="D70" t="n">
-        <v>2.17</v>
+        <v>0.64</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2073,76 +2073,76 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>10.343</v>
+        <v>17.782</v>
       </c>
       <c r="D72" t="n">
-        <v>5.69</v>
+        <v>1.5</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2.72</v>
+        <v>3.593</v>
       </c>
       <c r="D73" t="n">
-        <v>0.74</v>
+        <v>0.7</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D74" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2151,67 +2151,67 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>7.946</v>
+        <v>7.923</v>
       </c>
       <c r="D75" t="n">
-        <v>4.98</v>
+        <v>4.68</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>17.909</v>
+        <v>8.25</v>
       </c>
       <c r="D76" t="n">
-        <v>5.01</v>
+        <v>2.17</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.972</v>
+        <v>2.72</v>
       </c>
       <c r="D77" t="n">
-        <v>1.25</v>
+        <v>0.74</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2227,26 +2227,26 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Oct.17 2025    14:40</t>
+          <t>Oct.17 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6.187</v>
+        <v>1.086</v>
       </c>
       <c r="D79" t="n">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2257,65 +2257,65 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>17.055</v>
+        <v>18.7</v>
       </c>
       <c r="D80" t="n">
-        <v>3.36</v>
+        <v>0.64</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>18.7</v>
+        <v>1.086</v>
       </c>
       <c r="D81" t="n">
-        <v>0.64</v>
+        <v>0.93</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.972</v>
+        <v>3.593</v>
       </c>
       <c r="D82" t="n">
-        <v>1.25</v>
+        <v>0.7</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2326,19 +2326,19 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.086</v>
+        <v>6.187</v>
       </c>
       <c r="D83" t="n">
-        <v>0.93</v>
+        <v>0.03</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2349,180 +2349,180 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.522</v>
+        <v>8.25</v>
       </c>
       <c r="D84" t="n">
-        <v>4.2</v>
+        <v>2.17</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>23.833</v>
+        <v>138</v>
       </c>
       <c r="D85" t="n">
-        <v>1.42</v>
+        <v>-0.72</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>17.782</v>
+        <v>10.343</v>
       </c>
       <c r="D86" t="n">
-        <v>1.5</v>
+        <v>5.69</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>9.715</v>
+        <v>2.72</v>
       </c>
       <c r="D87" t="n">
-        <v>3.72</v>
+        <v>0.74</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>8.074999999999999</v>
+        <v>17.782</v>
       </c>
       <c r="D88" t="n">
-        <v>1.57</v>
+        <v>1.5</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2.7</v>
+        <v>7.946</v>
       </c>
       <c r="D89" t="n">
-        <v>1.89</v>
+        <v>4.98</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Oct.16 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>138</v>
+        <v>17.909</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.72</v>
+        <v>5.01</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3.593</v>
+        <v>0.972</v>
       </c>
       <c r="D91" t="n">
-        <v>0.7</v>
+        <v>1.25</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2533,42 +2533,42 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6.187</v>
+        <v>24.167</v>
       </c>
       <c r="D92" t="n">
-        <v>0.03</v>
+        <v>1.4</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.17 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.972</v>
+        <v>1.086</v>
       </c>
       <c r="D93" t="n">
-        <v>1.25</v>
+        <v>0.93</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2579,111 +2579,111 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>138</v>
+        <v>17.055</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.72</v>
+        <v>3.36</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>16.5</v>
+        <v>7.522</v>
       </c>
       <c r="D95" t="n">
-        <v>3.66</v>
+        <v>4.2</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>3.593</v>
+        <v>18.7</v>
       </c>
       <c r="D96" t="n">
-        <v>0.7</v>
+        <v>0.64</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>2.65</v>
+        <v>6.187</v>
       </c>
       <c r="D97" t="n">
-        <v>1.42</v>
+        <v>0.03</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1.086</v>
+        <v>3.593</v>
       </c>
       <c r="D98" t="n">
-        <v>0.93</v>
+        <v>0.7</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2694,19 +2694,19 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>18.7</v>
+        <v>138</v>
       </c>
       <c r="D99" t="n">
-        <v>0.64</v>
+        <v>-0.72</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2717,65 +2717,65 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>23.5</v>
+        <v>2.7</v>
       </c>
       <c r="D100" t="n">
-        <v>3.68</v>
+        <v>1.89</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>9.433</v>
+        <v>8.074999999999999</v>
       </c>
       <c r="D101" t="n">
-        <v>4.81</v>
+        <v>1.57</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>6.187</v>
+        <v>0.972</v>
       </c>
       <c r="D102" t="n">
-        <v>0.03</v>
+        <v>1.25</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2786,410 +2786,410 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>7.219</v>
+        <v>17.782</v>
       </c>
       <c r="D103" t="n">
-        <v>2.27</v>
+        <v>1.5</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>7.95</v>
+        <v>23.833</v>
       </c>
       <c r="D104" t="n">
-        <v>2.25</v>
+        <v>1.42</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Oct.15 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>17.782</v>
+        <v>9.715</v>
       </c>
       <c r="D105" t="n">
-        <v>1.5</v>
+        <v>3.72</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.16 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>2.613</v>
+        <v>23.5</v>
       </c>
       <c r="D106" t="n">
-        <v>0.5</v>
+        <v>3.68</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>9</v>
+        <v>0.972</v>
       </c>
       <c r="D107" t="n">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1.086</v>
+        <v>138</v>
       </c>
       <c r="D108" t="n">
-        <v>0.93</v>
+        <v>-0.72</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>3.593</v>
+        <v>16.5</v>
       </c>
       <c r="D109" t="n">
-        <v>0.7</v>
+        <v>3.66</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>18.7</v>
+        <v>3.593</v>
       </c>
       <c r="D110" t="n">
-        <v>0.64</v>
+        <v>0.7</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>17.782</v>
+        <v>2.65</v>
       </c>
       <c r="D111" t="n">
-        <v>1.5</v>
+        <v>1.42</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>7.775</v>
+        <v>1.086</v>
       </c>
       <c r="D112" t="n">
-        <v>0.65</v>
+        <v>0.93</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>7.059</v>
+        <v>18.7</v>
       </c>
       <c r="D113" t="n">
-        <v>0.79</v>
+        <v>0.64</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>138</v>
+        <v>9.433</v>
       </c>
       <c r="D114" t="n">
-        <v>-0.72</v>
+        <v>4.81</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15.918</v>
+        <v>6.187</v>
       </c>
       <c r="D115" t="n">
-        <v>1.8</v>
+        <v>0.03</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.972</v>
+        <v>7.219</v>
       </c>
       <c r="D116" t="n">
-        <v>1.25</v>
+        <v>2.27</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6.187</v>
+        <v>7.95</v>
       </c>
       <c r="D117" t="n">
-        <v>0.03</v>
+        <v>2.25</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.15 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>22.667</v>
+        <v>17.782</v>
       </c>
       <c r="D118" t="n">
-        <v>1.04</v>
+        <v>1.5</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Oct.14 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>18.7</v>
+        <v>2.613</v>
       </c>
       <c r="D119" t="n">
-        <v>0.64</v>
+        <v>0.5</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>3.593</v>
+        <v>1.086</v>
       </c>
       <c r="D120" t="n">
-        <v>0.7</v>
+        <v>0.93</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3200,99 +3200,99 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>22.433</v>
+        <v>9</v>
       </c>
       <c r="D121" t="n">
-        <v>3.14</v>
+        <v>1.5</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>0.972</v>
+        <v>22.667</v>
       </c>
       <c r="D122" t="n">
-        <v>1.25</v>
+        <v>1.04</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>7.004</v>
+        <v>6.187</v>
       </c>
       <c r="D123" t="n">
-        <v>2.16</v>
+        <v>0.03</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>8.867000000000001</v>
+        <v>0.972</v>
       </c>
       <c r="D124" t="n">
-        <v>3.38</v>
+        <v>1.25</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3301,21 +3301,21 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>15.636</v>
+        <v>15.918</v>
       </c>
       <c r="D125" t="n">
-        <v>2.75</v>
+        <v>1.8</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3338,122 +3338,122 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>17.782</v>
+        <v>7.059</v>
       </c>
       <c r="D127" t="n">
-        <v>1.5</v>
+        <v>0.79</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6.187</v>
+        <v>7.775</v>
       </c>
       <c r="D128" t="n">
-        <v>0.03</v>
+        <v>0.65</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.14 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1.086</v>
+        <v>17.782</v>
       </c>
       <c r="D129" t="n">
-        <v>0.93</v>
+        <v>1.5</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.6 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>2.6</v>
+        <v>18.7</v>
       </c>
       <c r="D130" t="n">
-        <v>0.97</v>
+        <v>0.64</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2025-10-13</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>7.725</v>
+        <v>3.593</v>
       </c>
       <c r="D131" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Oct.13 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3462,44 +3462,44 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.96</v>
+        <v>0.972</v>
       </c>
       <c r="D132" t="n">
-        <v>0.74</v>
+        <v>1.25</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>138</v>
+        <v>7.004</v>
       </c>
       <c r="D133" t="n">
-        <v>-0.72</v>
+        <v>2.16</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3522,53 +3522,53 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>7.663</v>
+        <v>22.433</v>
       </c>
       <c r="D135" t="n">
-        <v>0.5</v>
+        <v>3.14</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>2.575</v>
+        <v>3.593</v>
       </c>
       <c r="D136" t="n">
-        <v>2.47</v>
+        <v>0.7</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3577,217 +3577,217 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>8.577</v>
+        <v>8.867000000000001</v>
       </c>
       <c r="D137" t="n">
-        <v>1.23</v>
+        <v>3.38</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1.076</v>
+        <v>15.636</v>
       </c>
       <c r="D138" t="n">
-        <v>1.41</v>
+        <v>2.75</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>6.185</v>
+        <v>138</v>
       </c>
       <c r="D139" t="n">
-        <v>0.41</v>
+        <v>-0.72</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>3.568</v>
+        <v>17.782</v>
       </c>
       <c r="D140" t="n">
-        <v>0.68</v>
+        <v>1.5</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>21.75</v>
+        <v>6.187</v>
       </c>
       <c r="D141" t="n">
-        <v>1.52</v>
+        <v>0.03</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>17.782</v>
+        <v>1.086</v>
       </c>
       <c r="D142" t="n">
-        <v>1.5</v>
+        <v>0.93</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t xml:space="preserve">Oct.6 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>15.218</v>
+        <v>2.6</v>
       </c>
       <c r="D143" t="n">
-        <v>1.7</v>
+        <v>0.97</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-13</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>6.856</v>
+        <v>7.725</v>
       </c>
       <c r="D144" t="n">
-        <v>1.57</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Oct.10 2025    18:10</t>
+          <t>Oct.13 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>DDR3 4Gb 512Mx8 1600/1866</t>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>2.475</v>
+        <v>8.577</v>
       </c>
       <c r="D145" t="n">
-        <v>1.02</v>
+        <v>1.23</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>SLC 2Gb 256MBx8</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1.076</v>
+        <v>0.96</v>
       </c>
       <c r="D146" t="n">
-        <v>1.41</v>
+        <v>0.74</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -3798,249 +3798,249 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (2Gx8)3200</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>14.573</v>
+        <v>138</v>
       </c>
       <c r="D147" t="n">
-        <v>1.78</v>
+        <v>-0.72</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (512Mx16) 3200</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7.513</v>
+        <v>1.076</v>
       </c>
       <c r="D148" t="n">
-        <v>0.85</v>
+        <v>1.41</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>MLC 32Gb 4GBx8</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>3.568</v>
+        <v>18.7</v>
       </c>
       <c r="D149" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>DDR4 RDIMM 16GB 3200</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>138</v>
+        <v>7.663</v>
       </c>
       <c r="D150" t="n">
-        <v>-0.72</v>
+        <v>0.5</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>8.327999999999999</v>
+        <v>6.856</v>
       </c>
       <c r="D151" t="n">
-        <v>1.04</v>
+        <v>1.57</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>SLC 1Gb 128MBx8</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.96</v>
+        <v>15.218</v>
       </c>
       <c r="D152" t="n">
-        <v>0.74</v>
+        <v>1.7</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Sep.29 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>DDR4 16Gb (1Gx16)3200</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>21.188</v>
+        <v>17.782</v>
       </c>
       <c r="D153" t="n">
-        <v>0.71</v>
+        <v>1.5</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>DDR4 SODIMM 8GB 2666</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>18.7</v>
+        <v>21.75</v>
       </c>
       <c r="D154" t="n">
-        <v>0.64</v>
+        <v>1.52</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>DDR4 UDIMM 8GB 2666</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>17.782</v>
+        <v>2.575</v>
       </c>
       <c r="D155" t="n">
-        <v>1.5</v>
+        <v>2.47</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>Oct.6 2025    14:40</t>
+          <t>Oct.10 2025    18:10</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>DDR4 8Gb (1Gx8) 3200</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>6.584</v>
+        <v>6.185</v>
       </c>
       <c r="D156" t="n">
-        <v>0.61</v>
+        <v>0.41</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.8 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>MLC 64Gb 8GBx8</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>6.185</v>
+        <v>3.568</v>
       </c>
       <c r="D157" t="n">
-        <v>0.41</v>
+        <v>0.68</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4051,168 +4051,168 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 1Gb 128MBx8</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>7.949</v>
+        <v>0.96</v>
       </c>
       <c r="D158" t="n">
-        <v>0.9</v>
+        <v>0.74</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.2 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2025-10-01</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR3 4Gb 512Mx8 1600/1866</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7.816</v>
+        <v>2.475</v>
       </c>
       <c r="D159" t="n">
-        <v>1.82</v>
+        <v>1.02</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oct.1 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>SLC 2Gb 256MBx8</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7.573</v>
+        <v>1.076</v>
       </c>
       <c r="D160" t="n">
-        <v>0.5</v>
+        <v>1.41</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.30 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2025-09-29</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (2Gx8)3200</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>7.535</v>
+        <v>14.573</v>
       </c>
       <c r="D161" t="n">
-        <v>0.8</v>
+        <v>1.78</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.29 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (512Mx16) 3200</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>7.475</v>
+        <v>7.513</v>
       </c>
       <c r="D162" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.26 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2025-09-25</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 32Gb 4GBx8</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>7.349</v>
+        <v>3.568</v>
       </c>
       <c r="D163" t="n">
-        <v>2.21</v>
+        <v>0.68</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.25 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 RDIMM 16GB 3200</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>7.109</v>
+        <v>138</v>
       </c>
       <c r="D164" t="n">
-        <v>1.43</v>
+        <v>-0.72</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.24 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2025-09-23</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -4221,136 +4221,136 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>7.009</v>
+        <v>8.327999999999999</v>
       </c>
       <c r="D165" t="n">
-        <v>1.18</v>
+        <v>1.04</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.23 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2025-09-22</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 16Gb (1Gx16)3200</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>6.909</v>
+        <v>21.188</v>
       </c>
       <c r="D166" t="n">
-        <v>0.95</v>
+        <v>0.71</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.22 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 SODIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>6.776</v>
+        <v>18.7</v>
       </c>
       <c r="D167" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.19 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2025-09-18</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 UDIMM 8GB 2666</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>6.612</v>
+        <v>17.782</v>
       </c>
       <c r="D168" t="n">
-        <v>1.47</v>
+        <v>1.5</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.18 2025    14:40 </t>
+          <t>Oct.6 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2025-09-17</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>DDR4 8Gb (1Gx8) 3200</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>6.325</v>
+        <v>6.584</v>
       </c>
       <c r="D169" t="n">
-        <v>0.99</v>
+        <v>0.61</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.17 2025    14:40 </t>
+          <t xml:space="preserve">Oct.8 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-08</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>DDR5 16G (2Gx8) 4800/5600</t>
+          <t>MLC 64Gb 8GBx8</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>6.231</v>
+        <v>6.185</v>
       </c>
       <c r="D170" t="n">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sep.16 2025    14:40 </t>
+          <t>Sep.29 2025    14:40</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2025-09-15</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4359,21 +4359,21 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>6.216</v>
+        <v>7.949</v>
       </c>
       <c r="D171" t="n">
-        <v>0.26</v>
+        <v>0.9</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Sep.15 2025    14:39</t>
+          <t xml:space="preserve">Oct.2 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2025-09-12</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4382,21 +4382,21 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>6.2</v>
+        <v>7.816</v>
       </c>
       <c r="D172" t="n">
-        <v>1.09</v>
+        <v>1.82</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Sep.12 2025    14:38</t>
+          <t xml:space="preserve">Oct.1 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-30</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4405,21 +4405,21 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>6.083</v>
+        <v>7.573</v>
       </c>
       <c r="D173" t="n">
-        <v>0.26</v>
+        <v>0.5</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Sep.11 2025    14:37</t>
+          <t xml:space="preserve">Sep.30 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4428,21 +4428,21 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>6.05</v>
+        <v>7.535</v>
       </c>
       <c r="D174" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Sep.10 2025    14:36</t>
+          <t xml:space="preserve">Sep.29 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4451,21 +4451,21 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>6.05</v>
+        <v>7.475</v>
       </c>
       <c r="D175" t="n">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Sep.09 2025    14:36</t>
+          <t xml:space="preserve">Sep.26 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2025-09-08</t>
+          <t>2025-09-25</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4474,21 +4474,21 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>6.05</v>
+        <v>7.349</v>
       </c>
       <c r="D176" t="n">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Sep.08 2025    14:36</t>
+          <t xml:space="preserve">Sep.25 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2025-09-05</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4497,21 +4497,21 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>6.05</v>
+        <v>7.109</v>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>1.43</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Sep.05 2025    14:36</t>
+          <t xml:space="preserve">Sep.24 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2025-08-29</t>
+          <t>2025-09-23</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4520,21 +4520,21 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>6.17</v>
+        <v>7.009</v>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Aug.29 2025    14:36</t>
+          <t xml:space="preserve">Sep.23 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2025-08-28</t>
+          <t>2025-09-22</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4543,21 +4543,21 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>6.033</v>
+        <v>6.909</v>
       </c>
       <c r="D179" t="n">
-        <v>0.55</v>
+        <v>0.95</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Aug.28 2025    14:36</t>
+          <t xml:space="preserve">Sep.22 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2025-08-27</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -4566,21 +4566,21 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>5.967</v>
+        <v>6.776</v>
       </c>
       <c r="D180" t="n">
-        <v>-0.33</v>
+        <v>0.73</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Aug.27 2025    14:36</t>
+          <t xml:space="preserve">Sep.19 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2025-08-26</t>
+          <t>2025-09-18</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4589,21 +4589,21 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>6.017</v>
+        <v>6.612</v>
       </c>
       <c r="D181" t="n">
-        <v>-0.27</v>
+        <v>1.47</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Aug.26 2025    14:36</t>
+          <t xml:space="preserve">Sep.18 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2025-08-25</t>
+          <t>2025-09-17</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4612,21 +4612,21 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>6.033</v>
+        <v>6.325</v>
       </c>
       <c r="D182" t="n">
-        <v>-0.23</v>
+        <v>0.99</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Aug.25 2025    14:36</t>
+          <t xml:space="preserve">Sep.17 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2025-08-22</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4635,35 +4635,334 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6.05</v>
+        <v>6.231</v>
       </c>
       <c r="D183" t="n">
-        <v>-0.54</v>
+        <v>0.24</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Aug.22 2025    14:36</t>
+          <t xml:space="preserve">Sep.16 2025    14:40 </t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>6.216</v>
+      </c>
+      <c r="D184" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Sep.15 2025    14:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Sep.12 2025    14:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>6.083</v>
+      </c>
+      <c r="D186" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Sep.11 2025    14:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D187" t="n">
+        <v>0</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Sep.10 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D188" t="n">
+        <v>0</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Sep.09 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D189" t="n">
+        <v>0</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Sep.08 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D190" t="n">
+        <v>0</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Sep.05 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>6.17</v>
+      </c>
+      <c r="D191" t="n">
+        <v>0</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Aug.29 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D192" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Aug.28 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>5.967</v>
+      </c>
+      <c r="D193" t="n">
+        <v>-0.33</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Aug.27 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>6.017</v>
+      </c>
+      <c r="D194" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Aug.26 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>6.033</v>
+      </c>
+      <c r="D195" t="n">
+        <v>-0.23</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Aug.25 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>DDR5 16G (2Gx8) 4800/5600</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>6.05</v>
+      </c>
+      <c r="D196" t="n">
+        <v>-0.54</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Aug.22 2025    14:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
           <t>2025-08-19</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
+      <c r="B197" t="inlineStr">
         <is>
           <t>DDR5 16G (2Gx8) 4800/5600</t>
         </is>
       </c>
-      <c r="C184" t="n">
+      <c r="C197" t="n">
         <v>6.167</v>
       </c>
-      <c r="D184" t="n">
+      <c r="D197" t="n">
         <v>0</v>
       </c>
-      <c r="E184" t="inlineStr">
+      <c r="E197" t="inlineStr">
         <is>
           <t>Aug.19 2025    14:36</t>
         </is>

</xml_diff>